<commit_message>
commit para pasar a la laptop hp
</commit_message>
<xml_diff>
--- a/Exel apuntes/Libro1.xlsx
+++ b/Exel apuntes/Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darwi\Desktop\Jean Pierre\programacion\apuntes\Exel apuntes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B5A183-A9A2-4183-ADD8-9BB1EB978B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30E4DDC-499E-4EDE-8CA3-52179111A974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5844" yWindow="0" windowWidth="17292" windowHeight="12336" xr2:uid="{6DB1DB7E-0CB5-4A7E-9C7D-F63FF895EBF5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6DB1DB7E-0CB5-4A7E-9C7D-F63FF895EBF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="190">
   <si>
     <t>name</t>
   </si>
@@ -625,6 +625,12 @@
   </si>
   <si>
     <t>Gomez</t>
+  </si>
+  <si>
+    <t>Use la funcion split utilizada con la interfaz esta en: Datos/Herramientas de datos/Texto en columnas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es demasiado util para separar Datos mezcaldos </t>
   </si>
 </sst>
 </file>
@@ -635,7 +641,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;\-#,##0"/>
     <numFmt numFmtId="44" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -896,7 +902,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -934,34 +940,16 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -984,15 +972,12 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1023,6 +1008,24 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1184,25 +1187,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1231,6 +1215,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1238,111 +1231,72 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1380,17 +1334,20 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -1429,21 +1386,93 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1481,93 +1510,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -1962,6 +1905,66 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1976,28 +1979,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{106B28D2-7A29-464B-8D55-41387B9EA5BA}" name="tablaDeEjemplo" displayName="tablaDeEjemplo" ref="B3:L9" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76" totalsRowBorderDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{106B28D2-7A29-464B-8D55-41387B9EA5BA}" name="tablaDeEjemplo" displayName="tablaDeEjemplo" ref="B3:L9" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70" totalsRowBorderDxfId="69">
   <autoFilter ref="B3:L9" xr:uid="{106B28D2-7A29-464B-8D55-41387B9EA5BA}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{0137EC0B-8FC7-40DC-B7EA-C2233CDD3F9B}" name="name" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{97C5F091-3CFE-4438-8781-4838746115C9}" name="area" dataDxfId="73"/>
-    <tableColumn id="5" xr3:uid="{2239A232-9916-4280-A66E-EB49F23211B5}" name="ventas 1er trimestre" dataDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{371E5BCD-5E43-47A2-818B-3BCDB9AE0CCD}" name="ventas 2do trimestre" dataDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{E750F2FC-F469-4135-82F3-70B213AA432D}" name="vemtas 3er trimestre" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{A9460196-172B-4C8F-A5CB-002C198E83A9}" name="remarks 1er trimestre" dataDxfId="69">
+    <tableColumn id="1" xr3:uid="{0137EC0B-8FC7-40DC-B7EA-C2233CDD3F9B}" name="name" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{97C5F091-3CFE-4438-8781-4838746115C9}" name="area" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{2239A232-9916-4280-A66E-EB49F23211B5}" name="ventas 1er trimestre" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{371E5BCD-5E43-47A2-818B-3BCDB9AE0CCD}" name="ventas 2do trimestre" dataDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{E750F2FC-F469-4135-82F3-70B213AA432D}" name="vemtas 3er trimestre" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{A9460196-172B-4C8F-A5CB-002C198E83A9}" name="remarks 1er trimestre" dataDxfId="63">
       <calculatedColumnFormula>IF(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E8F30D65-30C9-4C55-849C-AD3671591B5C}" name="remarks 2do trimestre" dataDxfId="68">
+    <tableColumn id="7" xr3:uid="{E8F30D65-30C9-4C55-849C-AD3671591B5C}" name="remarks 2do trimestre" dataDxfId="62">
       <calculatedColumnFormula>IF(tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4ED204B2-A8F4-4B51-9CC9-335A974DF078}" name="remarks 3er trimestre" dataDxfId="67">
+    <tableColumn id="8" xr3:uid="{4ED204B2-A8F4-4B51-9CC9-335A974DF078}" name="remarks 3er trimestre" dataDxfId="61">
       <calculatedColumnFormula>IF(tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{883294BD-F0DE-4948-B10B-1449B22A6A4B}" name="ventas anuales 2022" dataDxfId="66">
+    <tableColumn id="9" xr3:uid="{883294BD-F0DE-4948-B10B-1449B22A6A4B}" name="ventas anuales 2022" dataDxfId="60">
       <calculatedColumnFormula>SUM(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]:[vemtas 3er trimestre]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{B6804E5B-F110-4CE5-904F-F2348926F4B6}" name="ventas anulaes 2021" dataDxfId="65"/>
-    <tableColumn id="12" xr3:uid="{7D0E706B-747E-475D-949D-BDCD1285CAE7}" name="trimestres perfectos" dataDxfId="64">
+    <tableColumn id="11" xr3:uid="{B6804E5B-F110-4CE5-904F-F2348926F4B6}" name="ventas anulaes 2021" dataDxfId="59"/>
+    <tableColumn id="12" xr3:uid="{7D0E706B-747E-475D-949D-BDCD1285CAE7}" name="trimestres perfectos" dataDxfId="58">
       <calculatedColumnFormula>IF(AND(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500),"beneficios en los tres trimestres","no hubo beneficios en todos los trimestres")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2006,11 +2009,11 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3D699D9-FFF9-41DF-9A82-0895F5359022}" name="Tabla911" displayName="Tabla911" ref="K121:L128" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3D699D9-FFF9-41DF-9A82-0895F5359022}" name="Tabla911" displayName="Tabla911" ref="K121:L128" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="K121:L128" xr:uid="{D3D699D9-FFF9-41DF-9A82-0895F5359022}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6370D7BF-23C4-435A-B977-1404D3A84FFE}" name="valor" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{B9EC1C73-CC5D-41BF-9E88-8CC9B95D208E}" name="rendodear min" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{6370D7BF-23C4-435A-B977-1404D3A84FFE}" name="valor" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{B9EC1C73-CC5D-41BF-9E88-8CC9B95D208E}" name="rendodear min" dataDxfId="17">
       <calculatedColumnFormula>ROUNDDOWN(Tabla911[[#This Row],[valor]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2019,10 +2022,10 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8026D621-F1C8-4D9D-A045-BE4AFFDBA19A}" name="Tabla11" displayName="Tabla11" ref="F138:L147" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8026D621-F1C8-4D9D-A045-BE4AFFDBA19A}" name="Tabla11" displayName="Tabla11" ref="F138:L147" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="F138:L147" xr:uid="{8026D621-F1C8-4D9D-A045-BE4AFFDBA19A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A77AB39D-26F4-47CC-A968-5047ECA883B3}" name="provincias" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{A77AB39D-26F4-47CC-A968-5047ECA883B3}" name="provincias" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{9A85997B-153C-45DC-BBDD-FCFE7A27825B}" name="mayuscula" dataDxfId="11">
       <calculatedColumnFormula>UPPER(Tabla11[[#This Row],[provincias]])</calculatedColumnFormula>
     </tableColumn>
@@ -2060,13 +2063,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6EB6F3A6-066B-448B-8745-4E445BD0AB3D}" name="Tabla6" displayName="Tabla6" ref="B21:E26" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6EB6F3A6-066B-448B-8745-4E445BD0AB3D}" name="Tabla6" displayName="Tabla6" ref="B21:E26" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <autoFilter ref="B21:E26" xr:uid="{6EB6F3A6-066B-448B-8745-4E445BD0AB3D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5E9E8327-50FB-4C88-82CF-5FD1E5175A06}" name="nombre" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{ACCF0C60-A980-4C3E-B22C-B4C68767939E}" name="ciudad" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{4D8D6F1E-6F34-4582-8616-980EE08CC19C}" name="edad" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{4107BD55-FF3B-4697-95B6-2F268DD3E983}" name="tipo" dataDxfId="58">
+    <tableColumn id="1" xr3:uid="{5E9E8327-50FB-4C88-82CF-5FD1E5175A06}" name="nombre" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{ACCF0C60-A980-4C3E-B22C-B4C68767939E}" name="ciudad" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{4D8D6F1E-6F34-4582-8616-980EE08CC19C}" name="edad" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{4107BD55-FF3B-4697-95B6-2F268DD3E983}" name="tipo" dataDxfId="52">
       <calculatedColumnFormula array="1">_xlfn.IFS(Tabla6[[#This Row],[edad]]&lt;=13,"niño",Tabla6[[#This Row],[edad]]&lt;=18,"adolecente",Tabla6[[#This Row],[edad]]&lt;=65,"joven adulto",Tabla6[[#This Row],[edad]]&gt;65,"tercera edad")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2075,36 +2078,36 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{34C047B8-B8C6-466E-9E71-6E7E426A73C6}" name="Tabla7" displayName="Tabla7" ref="G21:H25" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{34C047B8-B8C6-466E-9E71-6E7E426A73C6}" name="Tabla7" displayName="Tabla7" ref="G21:H25" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="G21:H25" xr:uid="{34C047B8-B8C6-466E-9E71-6E7E426A73C6}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CFABE698-2D63-49F2-A1F3-B643E7D7CD23}" name="edad" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{30963E77-7425-449A-8F48-DDDAEE82004D}" name="tipo" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{CFABE698-2D63-49F2-A1F3-B643E7D7CD23}" name="edad" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{30963E77-7425-449A-8F48-DDDAEE82004D}" name="tipo" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A56F233D-462B-4A5F-A4E9-3FA5F6DF8E3B}" name="Tabla1" displayName="Tabla1" ref="B33:E76" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A56F233D-462B-4A5F-A4E9-3FA5F6DF8E3B}" name="Tabla1" displayName="Tabla1" ref="B33:E76" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="B33:E76" xr:uid="{A56F233D-462B-4A5F-A4E9-3FA5F6DF8E3B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EA8A5CB7-15DD-4D25-960C-D74FCBEF1798}" name="mes" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{72E57F59-EBC6-42EB-8461-CE234EDFDC67}" name="vendedor" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{7773909E-A65A-453F-A426-5A342742EC9B}" name="ventas" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{C9E6D9A7-125C-4919-9494-287A09487570}" name="almacen" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{EA8A5CB7-15DD-4D25-960C-D74FCBEF1798}" name="mes" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{72E57F59-EBC6-42EB-8461-CE234EDFDC67}" name="vendedor" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{7773909E-A65A-453F-A426-5A342742EC9B}" name="ventas" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{C9E6D9A7-125C-4919-9494-287A09487570}" name="almacen" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E7FC109D-DC1F-4978-A063-14D5B4C9A387}" name="Tabla3" displayName="Tabla3" ref="B110:D115" totalsRowShown="0" headerRowDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E7FC109D-DC1F-4978-A063-14D5B4C9A387}" name="Tabla3" displayName="Tabla3" ref="B110:D115" totalsRowShown="0" headerRowDxfId="41">
   <autoFilter ref="B110:D115" xr:uid="{E7FC109D-DC1F-4978-A063-14D5B4C9A387}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{607690AB-B4D6-4244-880E-52F08CEE623D}" name="numero"/>
     <tableColumn id="2" xr3:uid="{AD175161-EE81-488E-9934-62D429B0D055}" name="divisor"/>
-    <tableColumn id="3" xr3:uid="{645960A9-E775-4F93-9587-209A231B1336}" name="residuo" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{645960A9-E775-4F93-9587-209A231B1336}" name="residuo" dataDxfId="40">
       <calculatedColumnFormula>MOD(Tabla3[[#This Row],[numero]],Tabla3[[#This Row],[divisor]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2113,7 +2116,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{358C82A8-4932-47BB-9305-0FBDE21DB47F}" name="Tabla4" displayName="Tabla4" ref="B83:E95" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="45" tableBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{358C82A8-4932-47BB-9305-0FBDE21DB47F}" name="Tabla4" displayName="Tabla4" ref="B83:E95" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37">
   <autoFilter ref="B83:E95" xr:uid="{AB8917A9-E925-4CE0-9F45-08618D9DA230}">
     <filterColumn colId="2">
       <filters>
@@ -2125,21 +2128,21 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E7702F9C-1406-4EC7-A2C6-E85CCFF4F3F1}" name="num" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{ED087E79-D309-4641-A64E-FB5C5EF15E96}" name="nombre de cliente" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{D32CEDAF-D0F3-4204-B879-F2AC4E8CBB7E}" name="inten vendido" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{5183FAAF-152C-480C-951E-AA05B61E558F}" name="ventas" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{E7702F9C-1406-4EC7-A2C6-E85CCFF4F3F1}" name="num" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{ED087E79-D309-4641-A64E-FB5C5EF15E96}" name="nombre de cliente" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{D32CEDAF-D0F3-4204-B879-F2AC4E8CBB7E}" name="inten vendido" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{5183FAAF-152C-480C-951E-AA05B61E558F}" name="ventas" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A7EAAFF8-9894-4E56-AD18-02049411D38C}" name="Tabla5" displayName="Tabla5" ref="B121:C124" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A7EAAFF8-9894-4E56-AD18-02049411D38C}" name="Tabla5" displayName="Tabla5" ref="B121:C124" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="B121:C124" xr:uid="{A7EAAFF8-9894-4E56-AD18-02049411D38C}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3678AD31-3C68-4D2F-94C5-37E335886AD8}" name="Vor"/>
-    <tableColumn id="2" xr3:uid="{4EC11E12-15D3-4B02-818E-9B9FBFCECE9F}" name="entero" dataDxfId="32">
+    <tableColumn id="2" xr3:uid="{4EC11E12-15D3-4B02-818E-9B9FBFCECE9F}" name="entero" dataDxfId="29">
       <calculatedColumnFormula>INT(Tabla5[[#This Row],[Vor]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2148,11 +2151,11 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CF10D987-1723-4933-81B3-0B77A1564462}" name="Tabla8" displayName="Tabla8" ref="E121:F124" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CF10D987-1723-4933-81B3-0B77A1564462}" name="Tabla8" displayName="Tabla8" ref="E121:F124" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26">
   <autoFilter ref="E121:F124" xr:uid="{CF10D987-1723-4933-81B3-0B77A1564462}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{31F71D3B-F428-4CBC-8609-DDC2C6F717F2}" name="valor"/>
-    <tableColumn id="2" xr3:uid="{2943EEA7-F064-4EF5-A236-C2A8E11F6D90}" name="3 decimales" dataDxfId="31">
+    <tableColumn id="2" xr3:uid="{2943EEA7-F064-4EF5-A236-C2A8E11F6D90}" name="3 decimales" dataDxfId="25">
       <calculatedColumnFormula>TRUNC(Tabla8[[#This Row],[valor]],3)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2161,11 +2164,11 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{24C98E62-6F10-4B70-9925-D3E6C668E51A}" name="Tabla9" displayName="Tabla9" ref="H121:I128" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{24C98E62-6F10-4B70-9925-D3E6C668E51A}" name="Tabla9" displayName="Tabla9" ref="H121:I128" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="H121:I128" xr:uid="{24C98E62-6F10-4B70-9925-D3E6C668E51A}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{89244227-8CDB-4E7A-8AE6-A60811A8E98D}" name="valor" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{FB930521-48C8-4A83-A824-96AB3D4C0B6C}" name="rendodear max" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{89244227-8CDB-4E7A-8AE6-A60811A8E98D}" name="valor" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{FB930521-48C8-4A83-A824-96AB3D4C0B6C}" name="rendodear max" dataDxfId="21">
       <calculatedColumnFormula>ROUNDUP(Tabla9[[#This Row],[valor]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2470,10 +2473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8917A9-E925-4CE0-9F45-08618D9DA230}">
-  <dimension ref="A2:L171"/>
+  <dimension ref="A2:L174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="46" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G143" sqref="G143"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="87" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2492,19 +2495,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
     </row>
     <row r="3" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
@@ -2770,11 +2773,11 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
@@ -2792,11 +2795,11 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -2923,11 +2926,11 @@
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
@@ -2959,10 +2962,10 @@
       <c r="J33" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="K33" s="13" t="s">
+      <c r="K33" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="L33" s="13"/>
+      <c r="L33" s="48"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
@@ -3173,10 +3176,10 @@
       <c r="J47" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="K47" s="14" t="s">
+      <c r="K47" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="L47" s="14"/>
+      <c r="L47" s="47"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B48" s="4" t="s">
@@ -3599,69 +3602,69 @@
         <f>POWER(B80,26)</f>
         <v>67108864</v>
       </c>
-      <c r="D80" s="13" t="s">
+      <c r="D80" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="E80" s="13"/>
+      <c r="E80" s="48"/>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B83" s="37" t="s">
+      <c r="B83" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C83" s="38" t="s">
+      <c r="C83" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D83" s="38" t="s">
+      <c r="D83" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="E83" s="39" t="s">
+      <c r="E83" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="F83" s="27" t="s">
+      <c r="F83" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="G83" s="28"/>
-      <c r="H83" s="28"/>
+      <c r="G83" s="50"/>
+      <c r="H83" s="50"/>
     </row>
     <row r="84" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="35">
+      <c r="B84" s="29">
         <v>5</v>
       </c>
-      <c r="C84" s="17" t="s">
+      <c r="C84" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D84" s="17" t="s">
+      <c r="D84" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E84" s="36">
+      <c r="E84" s="30">
         <v>1750</v>
       </c>
     </row>
     <row r="85" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="35">
+      <c r="B85" s="29">
         <v>12</v>
       </c>
-      <c r="C85" s="17" t="s">
+      <c r="C85" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D85" s="17" t="s">
+      <c r="D85" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E85" s="36">
+      <c r="E85" s="30">
         <v>452</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B86" s="35">
+      <c r="B86" s="29">
         <v>1</v>
       </c>
-      <c r="C86" s="17" t="s">
+      <c r="C86" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D86" s="17" t="s">
+      <c r="D86" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E86" s="36">
+      <c r="E86" s="30">
         <v>1100</v>
       </c>
       <c r="F86" t="s">
@@ -3669,16 +3672,16 @@
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B87" s="35">
+      <c r="B87" s="29">
         <v>8</v>
       </c>
-      <c r="C87" s="17" t="s">
+      <c r="C87" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D87" s="17" t="s">
+      <c r="D87" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E87" s="36">
+      <c r="E87" s="30">
         <v>1600</v>
       </c>
       <c r="F87" t="s">
@@ -3686,16 +3689,16 @@
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B88" s="35">
+      <c r="B88" s="29">
         <v>3</v>
       </c>
-      <c r="C88" s="17" t="s">
+      <c r="C88" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D88" s="17" t="s">
+      <c r="D88" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E88" s="36">
+      <c r="E88" s="30">
         <v>1750</v>
       </c>
       <c r="F88" t="s">
@@ -3703,16 +3706,16 @@
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B89" s="35">
+      <c r="B89" s="29">
         <v>9</v>
       </c>
-      <c r="C89" s="17" t="s">
+      <c r="C89" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D89" s="17" t="s">
+      <c r="D89" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E89" s="36">
+      <c r="E89" s="30">
         <v>350</v>
       </c>
       <c r="F89" t="s">
@@ -3720,16 +3723,16 @@
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B90" s="35">
+      <c r="B90" s="29">
         <v>2</v>
       </c>
-      <c r="C90" s="17" t="s">
+      <c r="C90" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D90" s="17" t="s">
+      <c r="D90" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E90" s="36">
+      <c r="E90" s="30">
         <v>1300</v>
       </c>
       <c r="F90" t="s">
@@ -3737,16 +3740,16 @@
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B91" s="35">
+      <c r="B91" s="29">
         <v>6</v>
       </c>
-      <c r="C91" s="17" t="s">
+      <c r="C91" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D91" s="17" t="s">
+      <c r="D91" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E91" s="36">
+      <c r="E91" s="30">
         <v>920</v>
       </c>
       <c r="F91" t="s">
@@ -3754,126 +3757,126 @@
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B92" s="35">
+      <c r="B92" s="29">
         <v>11</v>
       </c>
-      <c r="C92" s="17" t="s">
+      <c r="C92" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D92" s="17" t="s">
+      <c r="D92" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E92" s="36">
+      <c r="E92" s="30">
         <v>5650</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B93" s="35">
+      <c r="B93" s="29">
         <v>4</v>
       </c>
-      <c r="C93" s="17" t="s">
+      <c r="C93" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D93" s="17" t="s">
+      <c r="D93" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E93" s="36">
+      <c r="E93" s="30">
         <v>650</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B94" s="35">
+      <c r="B94" s="29">
         <v>7</v>
       </c>
-      <c r="C94" s="17" t="s">
+      <c r="C94" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D94" s="17" t="s">
+      <c r="D94" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E94" s="36">
+      <c r="E94" s="30">
         <v>235</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B95" s="35">
+      <c r="B95" s="29">
         <v>10</v>
       </c>
-      <c r="C95" s="17" t="s">
+      <c r="C95" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D95" s="22" t="s">
+      <c r="D95" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="E95" s="36">
+      <c r="E95" s="30">
         <v>250</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D96" s="23"/>
+      <c r="D96" s="19"/>
     </row>
     <row r="97" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C97" s="18" t="s">
+      <c r="C97" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="D97" s="19">
+      <c r="D97" s="15">
         <f>SUM(E84:E95)</f>
         <v>16007</v>
       </c>
     </row>
     <row r="98" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C98" s="20" t="s">
+      <c r="C98" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D98" s="21">
+      <c r="D98" s="17">
         <f>SUBTOTAL(9,E84:E95)</f>
         <v>13805</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C99" s="32" t="s">
+      <c r="C99" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="D99" s="29">
+      <c r="D99" s="23">
         <f>COUNT(B85:B95)</f>
         <v>11</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C100" s="33" t="s">
+      <c r="C100" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D100" s="30">
+      <c r="D100" s="24">
         <f>SUBTOTAL(2,B84:B95)</f>
         <v>10</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C101" s="32" t="s">
+      <c r="C101" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="D101" s="31">
+      <c r="D101" s="25">
         <f>AVERAGE(E86:E95)</f>
         <v>1380.5</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C102" s="33" t="s">
+      <c r="C102" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D102" s="30">
+      <c r="D102" s="24">
         <f>SUBTOTAL(1,E86:E95)</f>
         <v>1380.5</v>
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B110" s="34" t="s">
+      <c r="B110" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="C110" s="34" t="s">
+      <c r="C110" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="D110" s="34" t="s">
+      <c r="D110" s="28" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3938,23 +3941,22 @@
       </c>
     </row>
     <row r="117" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B117" s="13" t="s">
+      <c r="B117" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="C117" s="13"/>
+      <c r="C117" s="48"/>
     </row>
     <row r="121" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B121" s="40" t="s">
+      <c r="B121" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C121" s="40" t="s">
+      <c r="C121" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D121" s="41"/>
-      <c r="E121" s="40" t="s">
+      <c r="E121" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="F121" s="40" t="s">
+      <c r="F121" s="34" t="s">
         <v>115</v>
       </c>
       <c r="H121" s="4" t="s">
@@ -3971,18 +3973,17 @@
       </c>
     </row>
     <row r="122" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B122" s="41">
+      <c r="B122">
         <v>55.236521539999998</v>
       </c>
-      <c r="C122" s="41">
+      <c r="C122">
         <f>INT(Tabla5[[#This Row],[Vor]])</f>
         <v>55</v>
       </c>
-      <c r="D122" s="41"/>
-      <c r="E122" s="41">
+      <c r="E122">
         <v>55.236521539999998</v>
       </c>
-      <c r="F122" s="41">
+      <c r="F122">
         <f>TRUNC(Tabla8[[#This Row],[valor]],3)</f>
         <v>55.235999999999997</v>
       </c>
@@ -4002,18 +4003,17 @@
       </c>
     </row>
     <row r="123" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B123" s="41">
+      <c r="B123">
         <v>42.326598400000002</v>
       </c>
-      <c r="C123" s="41">
+      <c r="C123">
         <f>INT(Tabla5[[#This Row],[Vor]])</f>
         <v>42</v>
       </c>
-      <c r="D123" s="41"/>
-      <c r="E123" s="41">
+      <c r="E123">
         <v>42.326598400000002</v>
       </c>
-      <c r="F123" s="41">
+      <c r="F123">
         <f>TRUNC(Tabla8[[#This Row],[valor]],3)</f>
         <v>42.326000000000001</v>
       </c>
@@ -4033,18 +4033,17 @@
       </c>
     </row>
     <row r="124" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B124" s="41">
+      <c r="B124">
         <v>75.632564500000001</v>
       </c>
-      <c r="C124" s="41">
+      <c r="C124">
         <f>INT(Tabla5[[#This Row],[Vor]])</f>
         <v>75</v>
       </c>
-      <c r="D124" s="41"/>
-      <c r="E124" s="41">
+      <c r="E124">
         <v>75.632564500000001</v>
       </c>
-      <c r="F124" s="41">
+      <c r="F124">
         <f>TRUNC(Tabla8[[#This Row],[valor]],3)</f>
         <v>75.632000000000005</v>
       </c>
@@ -4080,14 +4079,14 @@
       </c>
     </row>
     <row r="126" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B126" s="13" t="s">
+      <c r="B126" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="C126" s="13"/>
-      <c r="E126" s="13" t="s">
+      <c r="C126" s="48"/>
+      <c r="E126" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="F126" s="13"/>
+      <c r="F126" s="48"/>
       <c r="H126" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -4136,666 +4135,681 @@
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H130" s="14" t="s">
+      <c r="H130" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="I130" s="14"/>
-      <c r="K130" s="13" t="s">
+      <c r="I130" s="47"/>
+      <c r="K130" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="L130" s="13"/>
+      <c r="L130" s="48"/>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B133" s="43" t="s">
+      <c r="B133" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="C133" s="43" t="s">
+      <c r="C133" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="D133" s="43" t="s">
+      <c r="D133" s="36" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B134" s="45">
+      <c r="B134" s="13">
         <v>75</v>
       </c>
-      <c r="C134" s="45">
+      <c r="C134" s="13">
         <v>84</v>
       </c>
-      <c r="D134" s="45">
+      <c r="D134" s="13">
         <v>58</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B135" s="45">
+      <c r="B135" s="13">
         <v>52</v>
       </c>
-      <c r="C135" s="45">
+      <c r="C135" s="13">
         <v>62</v>
       </c>
-      <c r="D135" s="45">
+      <c r="D135" s="13">
         <v>95</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B136" s="45">
+      <c r="B136" s="13">
         <v>65</v>
       </c>
-      <c r="C136" s="45">
+      <c r="C136" s="13">
         <v>53</v>
       </c>
-      <c r="D136" s="45">
+      <c r="D136" s="13">
         <v>72</v>
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B137" s="45">
+      <c r="B137" s="13">
         <v>84</v>
       </c>
-      <c r="C137" s="45">
+      <c r="C137" s="13">
         <v>48</v>
       </c>
-      <c r="D137" s="45">
+      <c r="D137" s="13">
         <v>16</v>
       </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B138" s="45">
+      <c r="B138" s="13">
         <v>45</v>
       </c>
-      <c r="C138" s="45">
+      <c r="C138" s="13">
         <v>85</v>
       </c>
-      <c r="D138" s="45">
+      <c r="D138" s="13">
         <v>48</v>
       </c>
-      <c r="F138" s="50" t="s">
+      <c r="F138" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="G138" s="51" t="s">
+      <c r="G138" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="H138" s="51" t="s">
+      <c r="H138" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="I138" s="52" t="s">
+      <c r="I138" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="J138" s="51" t="s">
+      <c r="J138" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="K138" s="51" t="s">
+      <c r="K138" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="L138" s="51" t="s">
+      <c r="L138" s="42" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B139" s="45">
+      <c r="B139" s="13">
         <v>25</v>
       </c>
-      <c r="C139" s="45">
+      <c r="C139" s="13">
         <v>96</v>
       </c>
-      <c r="D139" s="45">
+      <c r="D139" s="13">
         <v>29</v>
       </c>
-      <c r="F139" s="48" t="s">
+      <c r="F139" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="G139" s="46" t="str">
+      <c r="G139" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>PICHINCHA</v>
       </c>
-      <c r="H139" s="46" t="str">
+      <c r="H139" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>pichincha</v>
       </c>
-      <c r="I139" s="49">
+      <c r="I139" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>9</v>
       </c>
-      <c r="J139" s="25" t="str">
+      <c r="J139" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>pichincha</v>
       </c>
-      <c r="K139" s="24" t="str">
+      <c r="K139" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>pich</v>
       </c>
-      <c r="L139" s="25" t="str">
+      <c r="L139" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>*********</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B140" s="45">
+      <c r="B140" s="13">
         <v>74</v>
       </c>
-      <c r="C140" s="45">
+      <c r="C140" s="13">
         <v>75</v>
       </c>
-      <c r="D140" s="45">
+      <c r="D140" s="13">
         <v>75</v>
       </c>
-      <c r="F140" s="48" t="s">
+      <c r="F140" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="G140" s="46" t="str">
+      <c r="G140" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>GUAYAS</v>
       </c>
-      <c r="H140" s="46" t="str">
+      <c r="H140" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>guayas</v>
       </c>
-      <c r="I140" s="49">
+      <c r="I140" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>6</v>
       </c>
-      <c r="J140" s="25" t="str">
+      <c r="J140" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>guayas</v>
       </c>
-      <c r="K140" s="24" t="str">
+      <c r="K140" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>guay</v>
       </c>
-      <c r="L140" s="25" t="str">
+      <c r="L140" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>******</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B141" s="45">
+      <c r="B141" s="13">
         <v>63</v>
       </c>
-      <c r="C141" s="45">
+      <c r="C141" s="13">
         <v>48</v>
       </c>
-      <c r="D141" s="45">
+      <c r="D141" s="13">
         <v>36</v>
       </c>
-      <c r="F141" s="48" t="s">
+      <c r="F141" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G141" s="46" t="str">
+      <c r="G141" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>PASTAZA</v>
       </c>
-      <c r="H141" s="46" t="str">
+      <c r="H141" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>pastaza</v>
       </c>
-      <c r="I141" s="49">
+      <c r="I141" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>7</v>
       </c>
-      <c r="J141" s="25" t="str">
+      <c r="J141" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>pastaza</v>
       </c>
-      <c r="K141" s="24" t="str">
+      <c r="K141" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>past</v>
       </c>
-      <c r="L141" s="25" t="str">
+      <c r="L141" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>*******</v>
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B142" s="45">
+      <c r="B142" s="13">
         <v>35</v>
       </c>
-      <c r="C142" s="45">
+      <c r="C142" s="13">
         <v>28</v>
       </c>
-      <c r="D142" s="45">
+      <c r="D142" s="13">
         <v>25</v>
       </c>
-      <c r="F142" s="48" t="s">
+      <c r="F142" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="G142" s="46" t="str">
+      <c r="G142" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>ESMERALDAS</v>
       </c>
-      <c r="H142" s="46" t="str">
+      <c r="H142" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>esmeraldas</v>
       </c>
-      <c r="I142" s="49">
+      <c r="I142" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>10</v>
       </c>
-      <c r="J142" s="25" t="str">
+      <c r="J142" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>esmeraldas</v>
       </c>
-      <c r="K142" s="24" t="str">
+      <c r="K142" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>esme</v>
       </c>
-      <c r="L142" s="25" t="str">
+      <c r="L142" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>**********</v>
       </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B143" s="45">
+      <c r="B143" s="13">
         <v>25</v>
       </c>
-      <c r="C143" s="45">
+      <c r="C143" s="13">
         <v>95</v>
       </c>
-      <c r="D143" s="45">
+      <c r="D143" s="13">
         <v>42</v>
       </c>
-      <c r="F143" s="48" t="s">
+      <c r="F143" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="G143" s="46" t="str">
+      <c r="G143" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>LOS RIOS</v>
       </c>
-      <c r="H143" s="46" t="str">
+      <c r="H143" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>los rios</v>
       </c>
-      <c r="I143" s="49">
+      <c r="I143" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>8</v>
       </c>
-      <c r="J143" s="25" t="str">
+      <c r="J143" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>los rios</v>
       </c>
-      <c r="K143" s="24" t="str">
+      <c r="K143" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v xml:space="preserve">los </v>
       </c>
-      <c r="L143" s="25" t="str">
+      <c r="L143" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>********</v>
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A144" s="47" t="s">
+      <c r="A144" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="B144" s="26">
+      <c r="B144" s="22">
         <f>MAX(B134:B143)</f>
         <v>84</v>
       </c>
-      <c r="C144" s="26">
+      <c r="C144" s="22">
         <f>MAX(C134:C143)</f>
         <v>96</v>
       </c>
-      <c r="D144" s="26">
+      <c r="D144" s="22">
         <f>MAX(D134:D143)</f>
         <v>95</v>
       </c>
-      <c r="F144" s="48" t="s">
+      <c r="F144" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="G144" s="46" t="str">
+      <c r="G144" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>MANABI</v>
       </c>
-      <c r="H144" s="46" t="str">
+      <c r="H144" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>manabi</v>
       </c>
-      <c r="I144" s="49">
+      <c r="I144" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>6</v>
       </c>
-      <c r="J144" s="25" t="str">
+      <c r="J144" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>manabi</v>
       </c>
-      <c r="K144" s="24" t="str">
+      <c r="K144" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>mana</v>
       </c>
-      <c r="L144" s="25" t="str">
+      <c r="L144" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>******</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A145" s="47" t="s">
+      <c r="A145" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="B145" s="26">
+      <c r="B145" s="22">
         <f>MIN(B134:B143)</f>
         <v>25</v>
       </c>
-      <c r="C145" s="26">
+      <c r="C145" s="22">
         <f>MIN(C134:C143)</f>
         <v>28</v>
       </c>
-      <c r="D145" s="26">
+      <c r="D145" s="22">
         <f>MIN(D134:D143)</f>
         <v>16</v>
       </c>
-      <c r="F145" s="48" t="s">
+      <c r="F145" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="G145" s="46" t="str">
+      <c r="G145" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>LOJA</v>
       </c>
-      <c r="H145" s="46" t="str">
+      <c r="H145" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>loja</v>
       </c>
-      <c r="I145" s="49">
+      <c r="I145" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>4</v>
       </c>
-      <c r="J145" s="25" t="str">
+      <c r="J145" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>loja</v>
       </c>
-      <c r="K145" s="24" t="str">
+      <c r="K145" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>loja</v>
       </c>
-      <c r="L145" s="25" t="str">
+      <c r="L145" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>****</v>
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F146" s="48" t="s">
+      <c r="F146" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="G146" s="46" t="str">
+      <c r="G146" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>GALAPAGOS</v>
       </c>
-      <c r="H146" s="46" t="str">
+      <c r="H146" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>galapagos</v>
       </c>
-      <c r="I146" s="49">
+      <c r="I146" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>9</v>
       </c>
-      <c r="J146" s="25" t="str">
+      <c r="J146" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>galapagos</v>
       </c>
-      <c r="K146" s="24" t="str">
+      <c r="K146" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>gala</v>
       </c>
-      <c r="L146" s="25" t="str">
+      <c r="L146" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>*********</v>
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B147" s="13" t="s">
+      <c r="B147" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="C147" s="13"/>
-      <c r="F147" s="53" t="s">
+      <c r="C147" s="48"/>
+      <c r="F147" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="G147" s="54" t="str">
+      <c r="G147" s="45" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>SANTA ELENA</v>
       </c>
-      <c r="H147" s="54" t="str">
+      <c r="H147" s="45" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>santa elena</v>
       </c>
-      <c r="I147" s="55">
+      <c r="I147" s="46">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>11</v>
       </c>
-      <c r="J147" s="25" t="str">
+      <c r="J147" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>santa elena</v>
       </c>
-      <c r="K147" s="24" t="str">
+      <c r="K147" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>sant</v>
       </c>
-      <c r="L147" s="25" t="str">
+      <c r="L147" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>***********</v>
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B148" s="44" t="s">
+      <c r="B148" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B149" s="44" t="s">
+      <c r="B149" t="s">
         <v>126</v>
       </c>
-      <c r="F149" s="13" t="s">
+      <c r="F149" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="G149" s="13"/>
+      <c r="G149" s="48"/>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F150" s="44" t="s">
+      <c r="F150" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F151" s="44" t="s">
+      <c r="F151" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F152" s="44" t="s">
+      <c r="F152" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F153" s="23" t="s">
+      <c r="F153" s="19" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F154" s="44" t="s">
+      <c r="F154" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F155" s="44" t="s">
+      <c r="F155" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B162" s="42" t="s">
+    <row r="162" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B162" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="C162" s="42" t="s">
+      <c r="C162" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D162" s="42" t="s">
+      <c r="D162" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="E162" s="42" t="s">
+      <c r="E162" s="35" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B163" s="42" t="s">
+    <row r="163" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B163" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="C163" s="42" t="s">
+      <c r="C163" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="D163" s="42" t="s">
+      <c r="D163" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="E163" s="42" t="s">
+      <c r="E163" s="35" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B164" s="42" t="s">
+    <row r="164" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B164" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="C164" s="42" t="s">
+      <c r="C164" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="D164" s="42" t="s">
+      <c r="D164" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="E164" s="42" t="s">
+      <c r="E164" s="35" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B165" s="42" t="s">
+    <row r="165" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B165" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="C165" s="42" t="s">
+      <c r="C165" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="D165" s="42" t="s">
+      <c r="D165" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="E165" s="42" t="s">
+      <c r="E165" s="35" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="166" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B166" s="42" t="s">
+    <row r="166" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B166" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="C166" s="42" t="s">
+      <c r="C166" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="D166" s="42" t="s">
+      <c r="D166" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="E166" s="42" t="s">
+      <c r="E166" s="35" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="167" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B167" s="42" t="s">
+    <row r="167" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B167" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="C167" s="42" t="s">
+      <c r="C167" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="D167" s="42" t="s">
+      <c r="D167" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="E167" s="42" t="s">
+      <c r="E167" s="35" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="168" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B168" s="42" t="s">
+    <row r="168" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B168" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="C168" s="42" t="s">
+      <c r="C168" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="D168" s="42" t="s">
+      <c r="D168" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="E168" s="42" t="s">
+      <c r="E168" s="35" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="169" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B169" s="42" t="s">
+    <row r="169" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B169" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="C169" s="42" t="s">
+      <c r="C169" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="D169" s="42" t="s">
+      <c r="D169" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="E169" s="42" t="s">
+      <c r="E169" s="35" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B170" s="42" t="s">
+    <row r="170" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B170" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="C170" s="42" t="s">
+      <c r="C170" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="D170" s="42" t="s">
+      <c r="D170" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="E170" s="42" t="s">
+      <c r="E170" s="35" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="171" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B171" s="42" t="s">
+    <row r="171" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B171" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="C171" s="42" t="s">
+      <c r="C171" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="D171" s="42" t="s">
+      <c r="D171" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="E171" s="42" t="s">
+      <c r="E171" s="35" t="s">
         <v>187</v>
       </c>
     </row>
+    <row r="173" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B173" s="47" t="s">
+        <v>188</v>
+      </c>
+      <c r="C173" s="47"/>
+      <c r="D173" s="47"/>
+      <c r="E173" s="47"/>
+      <c r="F173" s="47"/>
+    </row>
+    <row r="174" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B174" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="H130:I130"/>
-    <mergeCell ref="K130:L130"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="F149:G149"/>
-    <mergeCell ref="F83:H83"/>
+  <mergeCells count="16">
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B173:F173"/>
     <mergeCell ref="D80:E80"/>
     <mergeCell ref="B117:C117"/>
     <mergeCell ref="B126:C126"/>
     <mergeCell ref="E126:F126"/>
     <mergeCell ref="K33:L33"/>
     <mergeCell ref="K47:L47"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="H130:I130"/>
+    <mergeCell ref="K130:L130"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="F149:G149"/>
+    <mergeCell ref="F83:H83"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="G4:J5">
-    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="hubo perdidas">
+    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="hubo perdidas">
       <formula>NOT(ISERROR(SEARCH("hubo perdidas",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="hubo perdidas">
+    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="hubo perdidas">
       <formula>NOT(ISERROR(SEARCH("hubo perdidas",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:J9">
-    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="hubo beneficios">
+    <cfRule type="containsText" dxfId="77" priority="3" operator="containsText" text="hubo beneficios">
       <formula>NOT(ISERROR(SEARCH("hubo beneficios",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="hubo perdidas">
+    <cfRule type="containsText" dxfId="76" priority="4" operator="containsText" text="hubo perdidas">
       <formula>NOT(ISERROR(SEARCH("hubo perdidas",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:L9">
-    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="no hubo beneficios en todos los trimestres">
+    <cfRule type="containsText" dxfId="75" priority="1" operator="containsText" text="no hubo beneficios en todos los trimestres">
       <formula>NOT(ISERROR(SEARCH("no hubo beneficios en todos los trimestres",L4)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="2" operator="equal">
       <formula>"beneficios en los tres trimestres"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
falta poco para terminar el curso de exel for begginers
</commit_message>
<xml_diff>
--- a/Exel apuntes/Libro1.xlsx
+++ b/Exel apuntes/Libro1.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darwi\Desktop\Jean Pierre\programacion\apuntes\Exel apuntes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanp\Videos\apuntes\Exel apuntes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30E4DDC-499E-4EDE-8CA3-52179111A974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4C1CD9-9908-47E1-B3A2-CD500BAD6871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6DB1DB7E-0CB5-4A7E-9C7D-F63FF895EBF5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6DB1DB7E-0CB5-4A7E-9C7D-F63FF895EBF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$83:$E$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$98:$E$110</definedName>
+    <definedName name="listaDinamicaDeElementos">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="227">
   <si>
     <t>name</t>
   </si>
@@ -631,6 +632,117 @@
   </si>
   <si>
     <t xml:space="preserve">Es demasiado util para separar Datos mezcaldos </t>
+  </si>
+  <si>
+    <t>NO. Fila</t>
+  </si>
+  <si>
+    <t>Nombre vendedor</t>
+  </si>
+  <si>
+    <t>Irma Polaco</t>
+  </si>
+  <si>
+    <t>Rafael Florez</t>
+  </si>
+  <si>
+    <t>Carlos Gonzales</t>
+  </si>
+  <si>
+    <t>Xiomara Vera</t>
+  </si>
+  <si>
+    <t>Alex Rodrigues</t>
+  </si>
+  <si>
+    <t>Nelson Ventura</t>
+  </si>
+  <si>
+    <t>Mayra Lopez</t>
+  </si>
+  <si>
+    <t>Lombardo Morales</t>
+  </si>
+  <si>
+    <t>$10,000.00</t>
+  </si>
+  <si>
+    <t>$20,000.00</t>
+  </si>
+  <si>
+    <t>$30,000.00</t>
+  </si>
+  <si>
+    <t>$40,000.00</t>
+  </si>
+  <si>
+    <t>$50,000.00</t>
+  </si>
+  <si>
+    <t>$60,000.00</t>
+  </si>
+  <si>
+    <t>$70,000.00</t>
+  </si>
+  <si>
+    <t>$80,000.00</t>
+  </si>
+  <si>
+    <t>$4,000.00</t>
+  </si>
+  <si>
+    <t>$446.00</t>
+  </si>
+  <si>
+    <t>$4,567.00</t>
+  </si>
+  <si>
+    <t>$5,664.00</t>
+  </si>
+  <si>
+    <t>$9,999.00</t>
+  </si>
+  <si>
+    <t>$433.00</t>
+  </si>
+  <si>
+    <t>$6,830.00</t>
+  </si>
+  <si>
+    <t>$891.00</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>nombre de vendedor</t>
+  </si>
+  <si>
+    <t>año de venta</t>
+  </si>
+  <si>
+    <t>valor a buscar</t>
+  </si>
+  <si>
+    <t>posicion del valor</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>jean-pi</t>
+  </si>
+  <si>
+    <t>Linkedin</t>
+  </si>
+  <si>
+    <t>Jean Pierre Veliz</t>
   </si>
 </sst>
 </file>
@@ -638,12 +750,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;\-#,##0"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;\-#,##0"/>
+    <numFmt numFmtId="165" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -695,8 +807,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -754,6 +881,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -898,16 +1031,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -937,14 +1071,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="6" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -952,14 +1086,14 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1014,24 +1148,121 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="87">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1386,7 +1617,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1525,7 +1756,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;\-#,##0"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;\-#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1710,7 +1941,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;\-#,##0"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;\-#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1905,66 +2136,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1979,28 +2150,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{106B28D2-7A29-464B-8D55-41387B9EA5BA}" name="tablaDeEjemplo" displayName="tablaDeEjemplo" ref="B3:L9" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70" totalsRowBorderDxfId="69">
-  <autoFilter ref="B3:L9" xr:uid="{106B28D2-7A29-464B-8D55-41387B9EA5BA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{106B28D2-7A29-464B-8D55-41387B9EA5BA}" name="tablaDeEjemplo" displayName="tablaDeEjemplo" ref="B18:L24" totalsRowShown="0" headerRowDxfId="86" dataDxfId="84" headerRowBorderDxfId="85" tableBorderDxfId="83" totalsRowBorderDxfId="82">
+  <autoFilter ref="B18:L24" xr:uid="{106B28D2-7A29-464B-8D55-41387B9EA5BA}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{0137EC0B-8FC7-40DC-B7EA-C2233CDD3F9B}" name="name" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{97C5F091-3CFE-4438-8781-4838746115C9}" name="area" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{2239A232-9916-4280-A66E-EB49F23211B5}" name="ventas 1er trimestre" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{371E5BCD-5E43-47A2-818B-3BCDB9AE0CCD}" name="ventas 2do trimestre" dataDxfId="65"/>
-    <tableColumn id="6" xr3:uid="{E750F2FC-F469-4135-82F3-70B213AA432D}" name="vemtas 3er trimestre" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{A9460196-172B-4C8F-A5CB-002C198E83A9}" name="remarks 1er trimestre" dataDxfId="63">
+    <tableColumn id="1" xr3:uid="{0137EC0B-8FC7-40DC-B7EA-C2233CDD3F9B}" name="name" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{97C5F091-3CFE-4438-8781-4838746115C9}" name="area" dataDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{2239A232-9916-4280-A66E-EB49F23211B5}" name="ventas 1er trimestre" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{371E5BCD-5E43-47A2-818B-3BCDB9AE0CCD}" name="ventas 2do trimestre" dataDxfId="78"/>
+    <tableColumn id="6" xr3:uid="{E750F2FC-F469-4135-82F3-70B213AA432D}" name="vemtas 3er trimestre" dataDxfId="77"/>
+    <tableColumn id="4" xr3:uid="{A9460196-172B-4C8F-A5CB-002C198E83A9}" name="remarks 1er trimestre" dataDxfId="76">
       <calculatedColumnFormula>IF(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E8F30D65-30C9-4C55-849C-AD3671591B5C}" name="remarks 2do trimestre" dataDxfId="62">
+    <tableColumn id="7" xr3:uid="{E8F30D65-30C9-4C55-849C-AD3671591B5C}" name="remarks 2do trimestre" dataDxfId="75">
       <calculatedColumnFormula>IF(tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4ED204B2-A8F4-4B51-9CC9-335A974DF078}" name="remarks 3er trimestre" dataDxfId="61">
+    <tableColumn id="8" xr3:uid="{4ED204B2-A8F4-4B51-9CC9-335A974DF078}" name="remarks 3er trimestre" dataDxfId="74">
       <calculatedColumnFormula>IF(tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{883294BD-F0DE-4948-B10B-1449B22A6A4B}" name="ventas anuales 2022" dataDxfId="60">
+    <tableColumn id="9" xr3:uid="{883294BD-F0DE-4948-B10B-1449B22A6A4B}" name="ventas anuales 2022" dataDxfId="73">
       <calculatedColumnFormula>SUM(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]:[vemtas 3er trimestre]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{B6804E5B-F110-4CE5-904F-F2348926F4B6}" name="ventas anulaes 2021" dataDxfId="59"/>
-    <tableColumn id="12" xr3:uid="{7D0E706B-747E-475D-949D-BDCD1285CAE7}" name="trimestres perfectos" dataDxfId="58">
+    <tableColumn id="11" xr3:uid="{B6804E5B-F110-4CE5-904F-F2348926F4B6}" name="ventas anulaes 2021" dataDxfId="72"/>
+    <tableColumn id="12" xr3:uid="{7D0E706B-747E-475D-949D-BDCD1285CAE7}" name="trimestres perfectos" dataDxfId="71">
       <calculatedColumnFormula>IF(AND(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500),"beneficios en los tres trimestres","no hubo beneficios en todos los trimestres")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2009,11 +2180,11 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3D699D9-FFF9-41DF-9A82-0895F5359022}" name="Tabla911" displayName="Tabla911" ref="K121:L128" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="K121:L128" xr:uid="{D3D699D9-FFF9-41DF-9A82-0895F5359022}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3D699D9-FFF9-41DF-9A82-0895F5359022}" name="Tabla911" displayName="Tabla911" ref="K136:L143" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="K136:L143" xr:uid="{D3D699D9-FFF9-41DF-9A82-0895F5359022}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6370D7BF-23C4-435A-B977-1404D3A84FFE}" name="valor" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{B9EC1C73-CC5D-41BF-9E88-8CC9B95D208E}" name="rendodear min" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{6370D7BF-23C4-435A-B977-1404D3A84FFE}" name="valor" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{B9EC1C73-CC5D-41BF-9E88-8CC9B95D208E}" name="rendodear min" dataDxfId="30">
       <calculatedColumnFormula>ROUNDDOWN(Tabla911[[#This Row],[valor]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2022,26 +2193,26 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8026D621-F1C8-4D9D-A045-BE4AFFDBA19A}" name="Tabla11" displayName="Tabla11" ref="F138:L147" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="F138:L147" xr:uid="{8026D621-F1C8-4D9D-A045-BE4AFFDBA19A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8026D621-F1C8-4D9D-A045-BE4AFFDBA19A}" name="Tabla11" displayName="Tabla11" ref="F153:L162" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="F153:L162" xr:uid="{8026D621-F1C8-4D9D-A045-BE4AFFDBA19A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A77AB39D-26F4-47CC-A968-5047ECA883B3}" name="provincias" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{9A85997B-153C-45DC-BBDD-FCFE7A27825B}" name="mayuscula" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{A77AB39D-26F4-47CC-A968-5047ECA883B3}" name="provincias" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{9A85997B-153C-45DC-BBDD-FCFE7A27825B}" name="mayuscula" dataDxfId="24">
       <calculatedColumnFormula>UPPER(Tabla11[[#This Row],[provincias]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A0FF24A8-7F7C-40BA-8DCB-CB21DAE09B5C}" name="minunculas" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{A0FF24A8-7F7C-40BA-8DCB-CB21DAE09B5C}" name="minunculas" dataDxfId="23">
       <calculatedColumnFormula>LOWER(Tabla11[[#This Row],[mayuscula]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{735277F2-0B8E-4F38-B429-CAE1289C4AE7}" name="num caracteres" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{735277F2-0B8E-4F38-B429-CAE1289C4AE7}" name="num caracteres" dataDxfId="22">
       <calculatedColumnFormula>LEN(Tabla11[[#This Row],[provincias]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A1794FC-73B0-4ABB-89F4-07B8458BEFE0}" name="elimina espacios" dataDxfId="8">
+    <tableColumn id="5" xr3:uid="{1A1794FC-73B0-4ABB-89F4-07B8458BEFE0}" name="elimina espacios" dataDxfId="21">
       <calculatedColumnFormula>TRIM(Tabla11[[#This Row],[provincias]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1A06D7DD-F336-457E-A41A-A360B702B51E}" name="Extrae 4 letras" dataDxfId="7">
+    <tableColumn id="6" xr3:uid="{1A06D7DD-F336-457E-A41A-A360B702B51E}" name="Extrae 4 letras" dataDxfId="20">
       <calculatedColumnFormula>MID(Tabla11[[#This Row],[provincias]],1,4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{60AAAA1E-9EB7-418A-B6C5-BCF3654A1854}" name="FUNCION REPT" dataDxfId="6">
+    <tableColumn id="7" xr3:uid="{60AAAA1E-9EB7-418A-B6C5-BCF3654A1854}" name="FUNCION REPT" dataDxfId="19">
       <calculatedColumnFormula>+REPT("*",Tabla11[[#This Row],[num caracteres]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2050,26 +2221,39 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{83B3A1EB-DFEE-40E1-A0E2-AB108A9AC8A4}" name="Tabla12" displayName="Tabla12" ref="B162:E171" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="B162:E171" xr:uid="{83B3A1EB-DFEE-40E1-A0E2-AB108A9AC8A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{83B3A1EB-DFEE-40E1-A0E2-AB108A9AC8A4}" name="Tabla12" displayName="Tabla12" ref="B177:E186" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="B177:E186" xr:uid="{83B3A1EB-DFEE-40E1-A0E2-AB108A9AC8A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{568943CD-A33E-4319-A345-796E5B3382FE}" name="Nombre y apellidos" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{2A7D9B85-CE83-4345-AF7D-0129B145E24B}" name="nombre" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{86D9DFB8-3D7C-4738-8E90-2A55D49E96FA}" name="primer apellido" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{9B9F10AD-C704-4D1D-AF2C-303FEF422ADD}" name="segundo apellido" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{568943CD-A33E-4319-A345-796E5B3382FE}" name="Nombre y apellidos" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{2A7D9B85-CE83-4345-AF7D-0129B145E24B}" name="nombre" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{86D9DFB8-3D7C-4738-8E90-2A55D49E96FA}" name="primer apellido" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{9B9F10AD-C704-4D1D-AF2C-303FEF422ADD}" name="segundo apellido" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{001BE3D0-530F-4C5C-BD63-52C228954A9D}" name="Tabla13" displayName="Tabla13" ref="H177:L185" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{3C1D4B05-F58D-4969-9F73-C2D47BCDCD6D}" name="NO. Fila" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{F9A00E65-91F8-45AC-AA23-51B1E281EEC1}" name="Nombre vendedor" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{2191A27F-0D06-46C4-BCDB-0DAEBC15C8CE}" name="2020" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{D1EA8C71-507E-4F2B-AA10-5C3A245CC3A2}" name="2021" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{DF693C14-5C57-4C54-8BFD-FFF9AB1F52FA}" name="2022" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6EB6F3A6-066B-448B-8745-4E445BD0AB3D}" name="Tabla6" displayName="Tabla6" ref="B21:E26" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
-  <autoFilter ref="B21:E26" xr:uid="{6EB6F3A6-066B-448B-8745-4E445BD0AB3D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6EB6F3A6-066B-448B-8745-4E445BD0AB3D}" name="Tabla6" displayName="Tabla6" ref="B36:E41" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
+  <autoFilter ref="B36:E41" xr:uid="{6EB6F3A6-066B-448B-8745-4E445BD0AB3D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5E9E8327-50FB-4C88-82CF-5FD1E5175A06}" name="nombre" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{ACCF0C60-A980-4C3E-B22C-B4C68767939E}" name="ciudad" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{4D8D6F1E-6F34-4582-8616-980EE08CC19C}" name="edad" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{4107BD55-FF3B-4697-95B6-2F268DD3E983}" name="tipo" dataDxfId="52">
+    <tableColumn id="1" xr3:uid="{5E9E8327-50FB-4C88-82CF-5FD1E5175A06}" name="nombre" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{ACCF0C60-A980-4C3E-B22C-B4C68767939E}" name="ciudad" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{4D8D6F1E-6F34-4582-8616-980EE08CC19C}" name="edad" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{4107BD55-FF3B-4697-95B6-2F268DD3E983}" name="tipo" dataDxfId="65">
       <calculatedColumnFormula array="1">_xlfn.IFS(Tabla6[[#This Row],[edad]]&lt;=13,"niño",Tabla6[[#This Row],[edad]]&lt;=18,"adolecente",Tabla6[[#This Row],[edad]]&lt;=65,"joven adulto",Tabla6[[#This Row],[edad]]&gt;65,"tercera edad")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2078,36 +2262,36 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{34C047B8-B8C6-466E-9E71-6E7E426A73C6}" name="Tabla7" displayName="Tabla7" ref="G21:H25" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
-  <autoFilter ref="G21:H25" xr:uid="{34C047B8-B8C6-466E-9E71-6E7E426A73C6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{34C047B8-B8C6-466E-9E71-6E7E426A73C6}" name="Tabla7" displayName="Tabla7" ref="G36:H40" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+  <autoFilter ref="G36:H40" xr:uid="{34C047B8-B8C6-466E-9E71-6E7E426A73C6}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CFABE698-2D63-49F2-A1F3-B643E7D7CD23}" name="edad" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{30963E77-7425-449A-8F48-DDDAEE82004D}" name="tipo" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{CFABE698-2D63-49F2-A1F3-B643E7D7CD23}" name="edad" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{30963E77-7425-449A-8F48-DDDAEE82004D}" name="tipo" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A56F233D-462B-4A5F-A4E9-3FA5F6DF8E3B}" name="Tabla1" displayName="Tabla1" ref="B33:E76" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
-  <autoFilter ref="B33:E76" xr:uid="{A56F233D-462B-4A5F-A4E9-3FA5F6DF8E3B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A56F233D-462B-4A5F-A4E9-3FA5F6DF8E3B}" name="Tabla1" displayName="Tabla1" ref="B48:E91" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+  <autoFilter ref="B48:E91" xr:uid="{A56F233D-462B-4A5F-A4E9-3FA5F6DF8E3B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EA8A5CB7-15DD-4D25-960C-D74FCBEF1798}" name="mes" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{72E57F59-EBC6-42EB-8461-CE234EDFDC67}" name="vendedor" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{7773909E-A65A-453F-A426-5A342742EC9B}" name="ventas" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{C9E6D9A7-125C-4919-9494-287A09487570}" name="almacen" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{EA8A5CB7-15DD-4D25-960C-D74FCBEF1798}" name="mes" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{72E57F59-EBC6-42EB-8461-CE234EDFDC67}" name="vendedor" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{7773909E-A65A-453F-A426-5A342742EC9B}" name="ventas" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{C9E6D9A7-125C-4919-9494-287A09487570}" name="almacen" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E7FC109D-DC1F-4978-A063-14D5B4C9A387}" name="Tabla3" displayName="Tabla3" ref="B110:D115" totalsRowShown="0" headerRowDxfId="41">
-  <autoFilter ref="B110:D115" xr:uid="{E7FC109D-DC1F-4978-A063-14D5B4C9A387}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E7FC109D-DC1F-4978-A063-14D5B4C9A387}" name="Tabla3" displayName="Tabla3" ref="B125:D130" totalsRowShown="0" headerRowDxfId="54">
+  <autoFilter ref="B125:D130" xr:uid="{E7FC109D-DC1F-4978-A063-14D5B4C9A387}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{607690AB-B4D6-4244-880E-52F08CEE623D}" name="numero"/>
     <tableColumn id="2" xr3:uid="{AD175161-EE81-488E-9934-62D429B0D055}" name="divisor"/>
-    <tableColumn id="3" xr3:uid="{645960A9-E775-4F93-9587-209A231B1336}" name="residuo" dataDxfId="40">
+    <tableColumn id="3" xr3:uid="{645960A9-E775-4F93-9587-209A231B1336}" name="residuo" dataDxfId="53">
       <calculatedColumnFormula>MOD(Tabla3[[#This Row],[numero]],Tabla3[[#This Row],[divisor]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2116,8 +2300,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{358C82A8-4932-47BB-9305-0FBDE21DB47F}" name="Tabla4" displayName="Tabla4" ref="B83:E95" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37">
-  <autoFilter ref="B83:E95" xr:uid="{AB8917A9-E925-4CE0-9F45-08618D9DA230}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{358C82A8-4932-47BB-9305-0FBDE21DB47F}" name="Tabla4" displayName="Tabla4" ref="B98:E110" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50">
+  <autoFilter ref="B98:E110" xr:uid="{AB8917A9-E925-4CE0-9F45-08618D9DA230}">
     <filterColumn colId="2">
       <filters>
         <filter val="Celular"/>
@@ -2128,21 +2312,21 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E7702F9C-1406-4EC7-A2C6-E85CCFF4F3F1}" name="num" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{ED087E79-D309-4641-A64E-FB5C5EF15E96}" name="nombre de cliente" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{D32CEDAF-D0F3-4204-B879-F2AC4E8CBB7E}" name="inten vendido" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{5183FAAF-152C-480C-951E-AA05B61E558F}" name="ventas" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{E7702F9C-1406-4EC7-A2C6-E85CCFF4F3F1}" name="num" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{ED087E79-D309-4641-A64E-FB5C5EF15E96}" name="nombre de cliente" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{D32CEDAF-D0F3-4204-B879-F2AC4E8CBB7E}" name="inten vendido" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{5183FAAF-152C-480C-951E-AA05B61E558F}" name="ventas" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A7EAAFF8-9894-4E56-AD18-02049411D38C}" name="Tabla5" displayName="Tabla5" ref="B121:C124" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30">
-  <autoFilter ref="B121:C124" xr:uid="{A7EAAFF8-9894-4E56-AD18-02049411D38C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A7EAAFF8-9894-4E56-AD18-02049411D38C}" name="Tabla5" displayName="Tabla5" ref="B136:C139" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43">
+  <autoFilter ref="B136:C139" xr:uid="{A7EAAFF8-9894-4E56-AD18-02049411D38C}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3678AD31-3C68-4D2F-94C5-37E335886AD8}" name="Vor"/>
-    <tableColumn id="2" xr3:uid="{4EC11E12-15D3-4B02-818E-9B9FBFCECE9F}" name="entero" dataDxfId="29">
+    <tableColumn id="2" xr3:uid="{4EC11E12-15D3-4B02-818E-9B9FBFCECE9F}" name="entero" dataDxfId="42">
       <calculatedColumnFormula>INT(Tabla5[[#This Row],[Vor]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2151,11 +2335,11 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CF10D987-1723-4933-81B3-0B77A1564462}" name="Tabla8" displayName="Tabla8" ref="E121:F124" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26">
-  <autoFilter ref="E121:F124" xr:uid="{CF10D987-1723-4933-81B3-0B77A1564462}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CF10D987-1723-4933-81B3-0B77A1564462}" name="Tabla8" displayName="Tabla8" ref="E136:F139" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39">
+  <autoFilter ref="E136:F139" xr:uid="{CF10D987-1723-4933-81B3-0B77A1564462}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{31F71D3B-F428-4CBC-8609-DDC2C6F717F2}" name="valor"/>
-    <tableColumn id="2" xr3:uid="{2943EEA7-F064-4EF5-A236-C2A8E11F6D90}" name="3 decimales" dataDxfId="25">
+    <tableColumn id="2" xr3:uid="{2943EEA7-F064-4EF5-A236-C2A8E11F6D90}" name="3 decimales" dataDxfId="38">
       <calculatedColumnFormula>TRUNC(Tabla8[[#This Row],[valor]],3)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2164,11 +2348,11 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{24C98E62-6F10-4B70-9925-D3E6C668E51A}" name="Tabla9" displayName="Tabla9" ref="H121:I128" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="H121:I128" xr:uid="{24C98E62-6F10-4B70-9925-D3E6C668E51A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{24C98E62-6F10-4B70-9925-D3E6C668E51A}" name="Tabla9" displayName="Tabla9" ref="H136:I143" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+  <autoFilter ref="H136:I143" xr:uid="{24C98E62-6F10-4B70-9925-D3E6C668E51A}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{89244227-8CDB-4E7A-8AE6-A60811A8E98D}" name="valor" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{FB930521-48C8-4A83-A824-96AB3D4C0B6C}" name="rendodear max" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{89244227-8CDB-4E7A-8AE6-A60811A8E98D}" name="valor" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{FB930521-48C8-4A83-A824-96AB3D4C0B6C}" name="rendodear max" dataDxfId="34">
       <calculatedColumnFormula>ROUNDUP(Tabla9[[#This Row],[valor]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2473,755 +2657,546 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8917A9-E925-4CE0-9F45-08618D9DA230}">
-  <dimension ref="A2:L174"/>
+  <dimension ref="A8:L189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="87" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B174" sqref="B174"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="I198" sqref="I198"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="8" width="15.77734375" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" customWidth="1"/>
-    <col min="12" max="12" width="25.88671875" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
+    <col min="12" max="12" width="25.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="51" t="s">
+    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>223</v>
+      </c>
+      <c r="E8" s="59" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-    </row>
-    <row r="3" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+    </row>
+    <row r="18" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L18" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+    <row r="19" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1">
         <v>10000</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E19" s="2">
         <v>4000</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F19" s="2">
         <v>4500</v>
       </c>
-      <c r="G4" s="3" t="str">
+      <c r="G19" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo beneficios</v>
       </c>
-      <c r="H4" s="3" t="str">
+      <c r="H19" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo beneficios</v>
       </c>
-      <c r="I4" s="3" t="str">
+      <c r="I19" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo beneficios</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J19" s="8">
         <f>SUM(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]:[vemtas 3er trimestre]])</f>
         <v>18500</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K19" s="8">
         <v>8500</v>
       </c>
-      <c r="L4" s="8" t="str">
+      <c r="L19" s="8" t="str">
         <f>IF(AND(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500),"beneficios en los tres trimestres","no hubo beneficios en todos los trimestres")</f>
         <v>beneficios en los tres trimestres</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+    <row r="20" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1">
         <v>5000</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E20" s="2">
         <v>2000</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F20" s="2">
         <v>2500</v>
       </c>
-      <c r="G5" s="3" t="str">
+      <c r="G20" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo beneficios</v>
       </c>
-      <c r="H5" s="3" t="str">
+      <c r="H20" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo perdidas</v>
       </c>
-      <c r="I5" s="3" t="str">
+      <c r="I20" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo perdidas</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J20" s="3">
         <f>SUM(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]:[vemtas 3er trimestre]])</f>
         <v>9500</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K20" s="3">
         <v>6000</v>
       </c>
-      <c r="L5" s="3" t="str">
+      <c r="L20" s="3" t="str">
         <f>IF(AND(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500),"beneficios en los tres trimestres","no hubo beneficios en todos los trimestres")</f>
         <v>no hubo beneficios en todos los trimestres</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+    <row r="21" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1">
         <v>6000</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E21" s="2">
         <v>6000</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F21" s="2">
         <v>1000</v>
       </c>
-      <c r="G6" s="3" t="str">
+      <c r="G21" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo beneficios</v>
       </c>
-      <c r="H6" s="3" t="str">
+      <c r="H21" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo beneficios</v>
       </c>
-      <c r="I6" s="3" t="str">
+      <c r="I21" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo perdidas</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J21" s="3">
         <f>SUM(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]:[vemtas 3er trimestre]])</f>
         <v>13000</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K21" s="3">
         <v>7000</v>
       </c>
-      <c r="L6" s="3" t="str">
+      <c r="L21" s="3" t="str">
         <f>IF(AND(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500),"beneficios en los tres trimestres","no hubo beneficios en todos los trimestres")</f>
         <v>no hubo beneficios en todos los trimestres</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+    <row r="22" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1">
         <v>15000</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E22" s="2">
         <v>5000</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F22" s="2">
         <v>5500</v>
       </c>
-      <c r="G7" s="3" t="str">
+      <c r="G22" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo beneficios</v>
       </c>
-      <c r="H7" s="3" t="str">
+      <c r="H22" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo beneficios</v>
       </c>
-      <c r="I7" s="3" t="str">
+      <c r="I22" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo beneficios</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J22" s="3">
         <f>SUM(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]:[vemtas 3er trimestre]])</f>
         <v>25500</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K22" s="3">
         <v>3500</v>
       </c>
-      <c r="L7" s="3" t="str">
+      <c r="L22" s="3" t="str">
         <f>IF(AND(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500),"beneficios en los tres trimestres","no hubo beneficios en todos los trimestres")</f>
         <v>beneficios en los tres trimestres</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+    <row r="23" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1">
         <v>35000</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E23" s="2">
         <v>10000</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F23" s="2">
         <v>4700</v>
       </c>
-      <c r="G8" s="3" t="str">
+      <c r="G23" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo beneficios</v>
       </c>
-      <c r="H8" s="3" t="str">
+      <c r="H23" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo beneficios</v>
       </c>
-      <c r="I8" s="3" t="str">
+      <c r="I23" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo beneficios</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J23" s="3">
         <f>SUM(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]:[vemtas 3er trimestre]])</f>
         <v>49700</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K23" s="3">
         <v>12000</v>
       </c>
-      <c r="L8" s="3" t="str">
+      <c r="L23" s="3" t="str">
         <f>IF(AND(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500),"beneficios en los tres trimestres","no hubo beneficios en todos los trimestres")</f>
         <v>beneficios en los tres trimestres</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+    <row r="24" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1">
         <v>2000</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E24" s="2">
         <v>1000</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F24" s="2">
         <v>3700</v>
       </c>
-      <c r="G9" s="3" t="str">
+      <c r="G24" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo perdidas</v>
       </c>
-      <c r="H9" s="3" t="str">
+      <c r="H24" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo perdidas</v>
       </c>
-      <c r="I9" s="3" t="str">
+      <c r="I24" s="3" t="str">
         <f>IF(tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500,"hubo beneficios","hubo perdidas")</f>
         <v>hubo beneficios</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J24" s="9">
         <f>SUM(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]:[vemtas 3er trimestre]])</f>
         <v>6700</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K24" s="9">
         <v>20000</v>
       </c>
-      <c r="L9" s="9" t="str">
+      <c r="L24" s="9" t="str">
         <f>IF(AND(tablaDeEjemplo[[#This Row],[ventas 1er trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[ventas 2do trimestre]]&gt;3500,tablaDeEjemplo[[#This Row],[vemtas 3er trimestre]]&gt;3500),"beneficios en los tres trimestres","no hubo beneficios en todos los trimestres")</f>
         <v>no hubo beneficios en todos los trimestres</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="48" t="s">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="52" t="s">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E36" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G36" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H36" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D37" s="4">
         <v>18</v>
       </c>
-      <c r="E22" s="10" t="str" cm="1">
-        <f t="array" ref="E22">_xlfn.IFS(Tabla6[[#This Row],[edad]]&lt;=13,"niño",Tabla6[[#This Row],[edad]]&lt;=18,"adolecente",Tabla6[[#This Row],[edad]]&lt;=65,"joven adulto",Tabla6[[#This Row],[edad]]&gt;65,"tercera edad")</f>
+      <c r="E37" s="10" t="str" cm="1">
+        <f t="array" ref="E37">_xlfn.IFS(Tabla6[[#This Row],[edad]]&lt;=13,"niño",Tabla6[[#This Row],[edad]]&lt;=18,"adolecente",Tabla6[[#This Row],[edad]]&lt;=65,"joven adulto",Tabla6[[#This Row],[edad]]&gt;65,"tercera edad")</f>
         <v>adolecente</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H37" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D38" s="4">
         <v>5</v>
       </c>
-      <c r="E23" s="4" t="str" cm="1">
-        <f t="array" ref="E23">_xlfn.IFS(Tabla6[[#This Row],[edad]]&lt;=13,"niño",Tabla6[[#This Row],[edad]]&lt;=18,"adolecente",Tabla6[[#This Row],[edad]]&lt;=65,"joven adulto",Tabla6[[#This Row],[edad]]&gt;65,"tercera edad")</f>
+      <c r="E38" s="4" t="str" cm="1">
+        <f t="array" ref="E38">_xlfn.IFS(Tabla6[[#This Row],[edad]]&lt;=13,"niño",Tabla6[[#This Row],[edad]]&lt;=18,"adolecente",Tabla6[[#This Row],[edad]]&lt;=65,"joven adulto",Tabla6[[#This Row],[edad]]&gt;65,"tercera edad")</f>
         <v>niño</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G38" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H38" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="4" t="s">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D39" s="4">
         <v>27</v>
       </c>
-      <c r="E24" s="4" t="str" cm="1">
-        <f t="array" ref="E24">_xlfn.IFS(Tabla6[[#This Row],[edad]]&lt;=13,"niño",Tabla6[[#This Row],[edad]]&lt;=18,"adolecente",Tabla6[[#This Row],[edad]]&lt;=65,"joven adulto",Tabla6[[#This Row],[edad]]&gt;65,"tercera edad")</f>
+      <c r="E39" s="4" t="str" cm="1">
+        <f t="array" ref="E39">_xlfn.IFS(Tabla6[[#This Row],[edad]]&lt;=13,"niño",Tabla6[[#This Row],[edad]]&lt;=18,"adolecente",Tabla6[[#This Row],[edad]]&lt;=65,"joven adulto",Tabla6[[#This Row],[edad]]&gt;65,"tercera edad")</f>
         <v>joven adulto</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G39" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H39" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="4" t="s">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D40" s="4">
         <v>70</v>
       </c>
-      <c r="E25" s="4" t="str" cm="1">
-        <f t="array" ref="E25">_xlfn.IFS(Tabla6[[#This Row],[edad]]&lt;=13,"niño",Tabla6[[#This Row],[edad]]&lt;=18,"adolecente",Tabla6[[#This Row],[edad]]&lt;=65,"joven adulto",Tabla6[[#This Row],[edad]]&gt;65,"tercera edad")</f>
+      <c r="E40" s="4" t="str" cm="1">
+        <f t="array" ref="E40">_xlfn.IFS(Tabla6[[#This Row],[edad]]&lt;=13,"niño",Tabla6[[#This Row],[edad]]&lt;=18,"adolecente",Tabla6[[#This Row],[edad]]&lt;=65,"joven adulto",Tabla6[[#This Row],[edad]]&gt;65,"tercera edad")</f>
         <v>tercera edad</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G40" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H40" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D41" s="4">
         <v>4</v>
       </c>
-      <c r="E26" s="4" t="str" cm="1">
-        <f t="array" ref="E26">_xlfn.IFS(Tabla6[[#This Row],[edad]]&lt;=13,"niño",Tabla6[[#This Row],[edad]]&lt;=18,"adolecente",Tabla6[[#This Row],[edad]]&lt;=65,"joven adulto",Tabla6[[#This Row],[edad]]&gt;65,"tercera edad")</f>
+      <c r="E41" s="4" t="str" cm="1">
+        <f t="array" ref="E41">_xlfn.IFS(Tabla6[[#This Row],[edad]]&lt;=13,"niño",Tabla6[[#This Row],[edad]]&lt;=18,"adolecente",Tabla6[[#This Row],[edad]]&lt;=65,"joven adulto",Tabla6[[#This Row],[edad]]&gt;65,"tercera edad")</f>
         <v>niño</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="47" t="s">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B33" s="11" t="s">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C48" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D48" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E48" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G48" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="H48" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I33" s="11" t="s">
+      <c r="I48" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="J33" s="11" t="s">
+      <c r="J48" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="K33" s="48" t="s">
+      <c r="K48" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="L33" s="48"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B34" s="4" t="s">
+      <c r="L48" s="48"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C49" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="D34" s="12">
-        <v>5000</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G34" s="10" t="str" cm="1">
-        <f t="array" ref="G34">_xlfn._xlws.FILTER(Tabla1[],Tabla1[mes]=G33,"no datos")</f>
-        <v>no datos</v>
-      </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B35" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="12">
-        <v>5000</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B36" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="12">
-        <v>3000</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B37" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="12">
-        <v>2500</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B38" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" s="12">
-        <v>3000</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B39" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="12">
-        <v>6200</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B40" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D40" s="12">
-        <v>4000</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="4"/>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B45" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="12">
-        <v>2500</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B46" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D46" s="12">
-        <v>5000</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B47" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D47" s="12">
-        <v>2500</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G47" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="I47" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="J47" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="K47" s="47" t="s">
-        <v>66</v>
-      </c>
-      <c r="L47" s="47"/>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B48" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D48" s="12">
-        <v>4000</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G48" t="str" cm="1">
-        <f t="array" ref="G48">_xlfn._xlws.FILTER(Tabla1[],(Tabla1[mes]=G47)*(Tabla1[vendedor]=H47),"no datos")</f>
-        <v>no datos</v>
-      </c>
-      <c r="K48" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="D49" s="12">
         <v>5000</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="G49" s="10" t="str" cm="1">
+        <f t="array" ref="G49">_xlfn._xlws.FILTER(Tabla1[],Tabla1[mes]=G48,"no datos")</f>
+        <v>no datos</v>
+      </c>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D50" s="12">
         <v>5000</v>
@@ -3229,167 +3204,159 @@
       <c r="E50" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="12">
+        <v>3000</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D51" s="12">
-        <v>4000</v>
-      </c>
-      <c r="E51" s="4" t="s">
+      <c r="C52" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="12">
+        <v>2500</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="4" t="s">
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D52" s="12">
-        <v>5000</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="C53" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D53" s="12">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D54" s="12">
-        <v>3000</v>
+        <v>6200</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D55" s="12">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C56" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D56" s="12">
-        <v>4000</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D57" s="12">
+      <c r="D60" s="12">
         <v>2500</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B58" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D58" s="12">
-        <v>5000</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B59" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D59" s="12">
-        <v>4000</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B60" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D60" s="12">
-        <v>5000</v>
-      </c>
       <c r="E60" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D61" s="12">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D62" s="12">
         <v>2500</v>
@@ -3397,10 +3364,26 @@
       <c r="E62" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G62" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H62" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I62" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J62" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K62" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="L62" s="47"/>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>59</v>
@@ -3409,152 +3392,159 @@
         <v>4000</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="G63" t="str" cm="1">
+        <f t="array" ref="G63">_xlfn._xlws.FILTER(Tabla1[],(Tabla1[mes]=G62)*(Tabla1[vendedor]=H62),"no datos")</f>
+        <v>no datos</v>
+      </c>
+      <c r="K63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D64" s="12">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D65" s="12">
+        <v>5000</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D66" s="12">
         <v>4000</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E66" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D67" s="12">
+        <v>5000</v>
+      </c>
+      <c r="E67" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B66" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D66" s="12">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D68" s="12">
         <v>5000</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E68" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B67" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D67" s="12">
-        <v>3000</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B68" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D68" s="12">
-        <v>2500</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D69" s="12">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D70" s="12">
         <v>5000</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D71" s="12">
+        <v>4000</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D72" s="12">
         <v>2500</v>
       </c>
-      <c r="E71" s="4" t="s">
+      <c r="E72" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B72" s="4" t="s">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D72" s="12">
-        <v>4000</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B73" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D73" s="12">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>56</v>
@@ -3563,1261 +3553,1637 @@
         <v>4000</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D75" s="12">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D76" s="12">
+        <v>3000</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="12">
+        <v>2500</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D78" s="12">
         <v>4000</v>
       </c>
-      <c r="E76" s="4" t="s">
+      <c r="E78" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D79" s="12">
+        <v>3000</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D80" s="12">
+        <v>4000</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D81" s="12">
+        <v>5000</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D82" s="12">
+        <v>3000</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D83" s="12">
+        <v>2500</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D84" s="12">
+        <v>4000</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D85" s="12">
+        <v>5000</v>
+      </c>
+      <c r="E85" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B80">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D86" s="12">
+        <v>2500</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D87" s="12">
+        <v>4000</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D88" s="12">
+        <v>3000</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D89" s="12">
+        <v>4000</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D90" s="12">
+        <v>2500</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D91" s="12">
+        <v>4000</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95">
         <v>2</v>
       </c>
-      <c r="C80">
-        <f>POWER(B80,26)</f>
+      <c r="C95">
+        <f>POWER(B95,26)</f>
         <v>67108864</v>
       </c>
-      <c r="D80" s="48" t="s">
+      <c r="D95" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="E80" s="48"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B83" s="31" t="s">
+      <c r="E95" s="48"/>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C83" s="32" t="s">
+      <c r="C98" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D83" s="32" t="s">
+      <c r="D98" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="E83" s="33" t="s">
+      <c r="E98" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="F83" s="49" t="s">
+      <c r="F98" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="G83" s="50"/>
-      <c r="H83" s="50"/>
-    </row>
-    <row r="84" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="29">
+      <c r="G98" s="52"/>
+      <c r="H98" s="52"/>
+    </row>
+    <row r="99" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="29">
         <v>5</v>
       </c>
-      <c r="C84" s="13" t="s">
+      <c r="C99" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D84" s="13" t="s">
+      <c r="D99" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E84" s="30">
+      <c r="E99" s="30">
         <v>1750</v>
       </c>
     </row>
-    <row r="85" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="29">
+    <row r="100" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="29">
         <v>12</v>
       </c>
-      <c r="C85" s="13" t="s">
+      <c r="C100" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D85" s="13" t="s">
+      <c r="D100" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E85" s="30">
+      <c r="E100" s="30">
         <v>452</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B86" s="29">
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="29">
         <v>1</v>
       </c>
-      <c r="C86" s="13" t="s">
+      <c r="C101" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D86" s="13" t="s">
+      <c r="D101" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E86" s="30">
+      <c r="E101" s="30">
         <v>1100</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F101" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B87" s="29">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="29">
         <v>8</v>
       </c>
-      <c r="C87" s="13" t="s">
+      <c r="C102" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D87" s="13" t="s">
+      <c r="D102" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E87" s="30">
+      <c r="E102" s="30">
         <v>1600</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F102" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B88" s="29">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B103" s="29">
         <v>3</v>
       </c>
-      <c r="C88" s="13" t="s">
+      <c r="C103" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D88" s="13" t="s">
+      <c r="D103" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E88" s="30">
+      <c r="E103" s="30">
         <v>1750</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F103" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B89" s="29">
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="29">
         <v>9</v>
       </c>
-      <c r="C89" s="13" t="s">
+      <c r="C104" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D89" s="13" t="s">
+      <c r="D104" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E89" s="30">
+      <c r="E104" s="30">
         <v>350</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F104" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B90" s="29">
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="29">
         <v>2</v>
       </c>
-      <c r="C90" s="13" t="s">
+      <c r="C105" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D90" s="13" t="s">
+      <c r="D105" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E90" s="30">
+      <c r="E105" s="30">
         <v>1300</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F105" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B91" s="29">
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="29">
         <v>6</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="C106" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D91" s="13" t="s">
+      <c r="D106" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E91" s="30">
+      <c r="E106" s="30">
         <v>920</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F106" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B92" s="29">
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="29">
         <v>11</v>
       </c>
-      <c r="C92" s="13" t="s">
+      <c r="C107" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D92" s="13" t="s">
+      <c r="D107" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E92" s="30">
+      <c r="E107" s="30">
         <v>5650</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B93" s="29">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B108" s="29">
         <v>4</v>
       </c>
-      <c r="C93" s="13" t="s">
+      <c r="C108" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D93" s="13" t="s">
+      <c r="D108" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E93" s="30">
+      <c r="E108" s="30">
         <v>650</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B94" s="29">
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B109" s="29">
         <v>7</v>
       </c>
-      <c r="C94" s="13" t="s">
+      <c r="C109" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D94" s="13" t="s">
+      <c r="D109" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E94" s="30">
+      <c r="E109" s="30">
         <v>235</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B95" s="29">
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B110" s="29">
         <v>10</v>
       </c>
-      <c r="C95" s="13" t="s">
+      <c r="C110" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D95" s="18" t="s">
+      <c r="D110" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="E95" s="30">
+      <c r="E110" s="30">
         <v>250</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D96" s="19"/>
-    </row>
-    <row r="97" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C97" s="14" t="s">
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D111" s="19"/>
+    </row>
+    <row r="112" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C112" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="D97" s="15">
-        <f>SUM(E84:E95)</f>
+      <c r="D112" s="15">
+        <f>SUM(E99:E110)</f>
         <v>16007</v>
       </c>
     </row>
-    <row r="98" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C98" s="16" t="s">
+    <row r="113" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C113" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D98" s="17">
-        <f>SUBTOTAL(9,E84:E95)</f>
+      <c r="D113" s="17">
+        <f>SUBTOTAL(9,E99:E110)</f>
         <v>13805</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C99" s="26" t="s">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C114" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="D99" s="23">
-        <f>COUNT(B85:B95)</f>
+      <c r="D114" s="23">
+        <f>COUNT(B100:B110)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C100" s="27" t="s">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C115" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D100" s="24">
-        <f>SUBTOTAL(2,B84:B95)</f>
+      <c r="D115" s="24">
+        <f>SUBTOTAL(2,B99:B110)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C101" s="26" t="s">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C116" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="D101" s="25">
-        <f>AVERAGE(E86:E95)</f>
+      <c r="D116" s="25">
+        <f>AVERAGE(E101:E110)</f>
         <v>1380.5</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C102" s="27" t="s">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C117" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D102" s="24">
-        <f>SUBTOTAL(1,E86:E95)</f>
+      <c r="D117" s="24">
+        <f>SUBTOTAL(1,E101:E110)</f>
         <v>1380.5</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B110" s="28" t="s">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="C110" s="28" t="s">
+      <c r="C125" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="D110" s="28" t="s">
+      <c r="D125" s="28" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B111">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B126">
         <v>8</v>
       </c>
-      <c r="C111">
+      <c r="C126">
         <v>9</v>
       </c>
-      <c r="D111">
+      <c r="D126">
         <f>MOD(Tabla3[[#This Row],[numero]],Tabla3[[#This Row],[divisor]])</f>
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B112">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B127">
         <v>5</v>
       </c>
-      <c r="C112">
+      <c r="C127">
         <v>20</v>
       </c>
-      <c r="D112">
+      <c r="D127">
         <f>MOD(Tabla3[[#This Row],[numero]],Tabla3[[#This Row],[divisor]])</f>
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B113">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B128">
         <v>2</v>
       </c>
-      <c r="C113">
+      <c r="C128">
         <v>8</v>
       </c>
-      <c r="D113">
+      <c r="D128">
         <f>MOD(Tabla3[[#This Row],[numero]],Tabla3[[#This Row],[divisor]])</f>
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B114">
+    <row r="129" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B129">
         <v>4</v>
       </c>
-      <c r="C114">
+      <c r="C129">
         <v>9</v>
       </c>
-      <c r="D114">
+      <c r="D129">
         <f>MOD(Tabla3[[#This Row],[numero]],Tabla3[[#This Row],[divisor]])</f>
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B115">
+    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B130">
         <v>7</v>
       </c>
-      <c r="C115">
+      <c r="C130">
         <v>5</v>
       </c>
-      <c r="D115">
+      <c r="D130">
         <f>MOD(Tabla3[[#This Row],[numero]],Tabla3[[#This Row],[divisor]])</f>
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B117" s="48" t="s">
+    <row r="132" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B132" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="C117" s="48"/>
-    </row>
-    <row r="121" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B121" s="34" t="s">
+      <c r="C132" s="48"/>
+    </row>
+    <row r="136" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B136" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C121" s="34" t="s">
+      <c r="C136" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="E121" s="34" t="s">
+      <c r="E136" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="F121" s="34" t="s">
+      <c r="F136" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="H121" s="4" t="s">
+      <c r="H136" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="I121" s="4" t="s">
+      <c r="I136" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="K121" s="4" t="s">
+      <c r="K136" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="L121" s="4" t="s">
+      <c r="L136" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B122">
+    <row r="137" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B137">
         <v>55.236521539999998</v>
       </c>
-      <c r="C122">
+      <c r="C137">
         <f>INT(Tabla5[[#This Row],[Vor]])</f>
         <v>55</v>
       </c>
-      <c r="E122">
+      <c r="E137">
         <v>55.236521539999998</v>
       </c>
-      <c r="F122">
+      <c r="F137">
         <f>TRUNC(Tabla8[[#This Row],[valor]],3)</f>
         <v>55.235999999999997</v>
       </c>
-      <c r="H122" s="4">
+      <c r="H137" s="4">
         <v>2.2456399999999999</v>
       </c>
-      <c r="I122" s="4">
+      <c r="I137" s="4">
         <f>ROUNDUP(Tabla9[[#This Row],[valor]],0)</f>
         <v>3</v>
       </c>
-      <c r="K122" s="4">
+      <c r="K137" s="4">
         <v>2.2456399999999999</v>
       </c>
-      <c r="L122" s="4">
+      <c r="L137" s="4">
         <f>ROUNDDOWN(Tabla911[[#This Row],[valor]],0)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B123">
+    <row r="138" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B138">
         <v>42.326598400000002</v>
       </c>
-      <c r="C123">
+      <c r="C138">
         <f>INT(Tabla5[[#This Row],[Vor]])</f>
         <v>42</v>
       </c>
-      <c r="E123">
+      <c r="E138">
         <v>42.326598400000002</v>
       </c>
-      <c r="F123">
+      <c r="F138">
         <f>TRUNC(Tabla8[[#This Row],[valor]],3)</f>
         <v>42.326000000000001</v>
       </c>
-      <c r="H123" s="4">
+      <c r="H138" s="4">
         <v>3.9867565420000002</v>
       </c>
-      <c r="I123" s="4">
+      <c r="I138" s="4">
         <f>ROUNDUP(Tabla9[[#This Row],[valor]],0)</f>
         <v>4</v>
       </c>
-      <c r="K123" s="4">
+      <c r="K138" s="4">
         <v>3.9867565420000002</v>
       </c>
-      <c r="L123" s="4">
+      <c r="L138" s="4">
         <f>ROUNDDOWN(Tabla911[[#This Row],[valor]],0)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B124">
+    <row r="139" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B139">
         <v>75.632564500000001</v>
       </c>
-      <c r="C124">
+      <c r="C139">
         <f>INT(Tabla5[[#This Row],[Vor]])</f>
         <v>75</v>
       </c>
-      <c r="E124">
+      <c r="E139">
         <v>75.632564500000001</v>
       </c>
-      <c r="F124">
+      <c r="F139">
         <f>TRUNC(Tabla8[[#This Row],[valor]],3)</f>
         <v>75.632000000000005</v>
       </c>
-      <c r="H124" s="4">
+      <c r="H139" s="4">
         <v>6.21</v>
       </c>
-      <c r="I124" s="4">
+      <c r="I139" s="4">
         <f>ROUNDUP(Tabla9[[#This Row],[valor]],0)</f>
         <v>7</v>
       </c>
-      <c r="K124" s="4">
+      <c r="K139" s="4">
         <v>6.21</v>
       </c>
-      <c r="L124" s="4">
+      <c r="L139" s="4">
         <f>ROUNDDOWN(Tabla911[[#This Row],[valor]],0)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="H125" s="4">
+    <row r="140" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H140" s="4">
         <v>6.0339999999999998</v>
       </c>
-      <c r="I125" s="4">
+      <c r="I140" s="4">
         <f>ROUNDUP(Tabla9[[#This Row],[valor]],0)</f>
         <v>7</v>
       </c>
-      <c r="K125" s="4">
+      <c r="K140" s="4">
         <v>6.0339999999999998</v>
       </c>
-      <c r="L125" s="4">
+      <c r="L140" s="4">
         <f>ROUNDDOWN(Tabla911[[#This Row],[valor]],0)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B126" s="48" t="s">
+    <row r="141" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B141" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="C126" s="48"/>
-      <c r="E126" s="48" t="s">
+      <c r="C141" s="48"/>
+      <c r="E141" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="F126" s="48"/>
-      <c r="H126" s="4">
+      <c r="F141" s="48"/>
+      <c r="H141" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I126" s="4">
+      <c r="I141" s="4">
         <f>ROUNDUP(Tabla9[[#This Row],[valor]],0)</f>
         <v>2</v>
       </c>
-      <c r="K126" s="4">
+      <c r="K141" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L126" s="4">
+      <c r="L141" s="4">
         <f>ROUNDDOWN(Tabla911[[#This Row],[valor]],0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="H127" s="4">
+    <row r="142" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H142" s="4">
         <v>6.8</v>
       </c>
-      <c r="I127" s="4">
+      <c r="I142" s="4">
         <f>ROUNDUP(Tabla9[[#This Row],[valor]],0)</f>
         <v>7</v>
       </c>
-      <c r="K127" s="4">
+      <c r="K142" s="4">
         <v>6.8</v>
       </c>
-      <c r="L127" s="4">
+      <c r="L142" s="4">
         <f>ROUNDDOWN(Tabla911[[#This Row],[valor]],0)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="128" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="H128" s="4">
+    <row r="143" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H143" s="4">
         <v>4.5</v>
       </c>
-      <c r="I128" s="4">
+      <c r="I143" s="4">
         <f>ROUNDUP(Tabla9[[#This Row],[valor]],0)</f>
         <v>5</v>
       </c>
-      <c r="K128" s="4">
+      <c r="K143" s="4">
         <v>4.5</v>
       </c>
-      <c r="L128" s="4">
+      <c r="L143" s="4">
         <f>ROUNDDOWN(Tabla911[[#This Row],[valor]],0)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H130" s="47" t="s">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H145" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="I130" s="47"/>
-      <c r="K130" s="48" t="s">
+      <c r="I145" s="47"/>
+      <c r="K145" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="L130" s="48"/>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B133" s="36" t="s">
+      <c r="L145" s="48"/>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B148" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="C133" s="36" t="s">
+      <c r="C148" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="D133" s="36" t="s">
+      <c r="D148" s="36" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B134" s="13">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B149" s="13">
         <v>75</v>
       </c>
-      <c r="C134" s="13">
+      <c r="C149" s="13">
         <v>84</v>
       </c>
-      <c r="D134" s="13">
+      <c r="D149" s="13">
         <v>58</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B135" s="13">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B150" s="13">
         <v>52</v>
       </c>
-      <c r="C135" s="13">
+      <c r="C150" s="13">
         <v>62</v>
       </c>
-      <c r="D135" s="13">
+      <c r="D150" s="13">
         <v>95</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B136" s="13">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B151" s="13">
         <v>65</v>
       </c>
-      <c r="C136" s="13">
+      <c r="C151" s="13">
         <v>53</v>
       </c>
-      <c r="D136" s="13">
+      <c r="D151" s="13">
         <v>72</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B137" s="13">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B152" s="13">
         <v>84</v>
       </c>
-      <c r="C137" s="13">
+      <c r="C152" s="13">
         <v>48</v>
       </c>
-      <c r="D137" s="13">
+      <c r="D152" s="13">
         <v>16</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B138" s="13">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B153" s="13">
         <v>45</v>
       </c>
-      <c r="C138" s="13">
+      <c r="C153" s="13">
         <v>85</v>
       </c>
-      <c r="D138" s="13">
+      <c r="D153" s="13">
         <v>48</v>
       </c>
-      <c r="F138" s="41" t="s">
+      <c r="F153" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="G138" s="42" t="s">
+      <c r="G153" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="H138" s="42" t="s">
+      <c r="H153" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="I138" s="43" t="s">
+      <c r="I153" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="J138" s="42" t="s">
+      <c r="J153" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="K138" s="42" t="s">
+      <c r="K153" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="L138" s="42" t="s">
+      <c r="L153" s="42" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B139" s="13">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B154" s="13">
         <v>25</v>
       </c>
-      <c r="C139" s="13">
+      <c r="C154" s="13">
         <v>96</v>
       </c>
-      <c r="D139" s="13">
+      <c r="D154" s="13">
         <v>29</v>
       </c>
-      <c r="F139" s="39" t="s">
+      <c r="F154" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="G139" s="37" t="str">
+      <c r="G154" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>PICHINCHA</v>
       </c>
-      <c r="H139" s="37" t="str">
+      <c r="H154" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>pichincha</v>
       </c>
-      <c r="I139" s="40">
+      <c r="I154" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>9</v>
       </c>
-      <c r="J139" s="21" t="str">
+      <c r="J154" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>pichincha</v>
       </c>
-      <c r="K139" s="20" t="str">
+      <c r="K154" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>pich</v>
       </c>
-      <c r="L139" s="21" t="str">
+      <c r="L154" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>*********</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B140" s="13">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B155" s="13">
         <v>74</v>
       </c>
-      <c r="C140" s="13">
+      <c r="C155" s="13">
         <v>75</v>
       </c>
-      <c r="D140" s="13">
+      <c r="D155" s="13">
         <v>75</v>
       </c>
-      <c r="F140" s="39" t="s">
+      <c r="F155" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="G140" s="37" t="str">
+      <c r="G155" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>GUAYAS</v>
       </c>
-      <c r="H140" s="37" t="str">
+      <c r="H155" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>guayas</v>
       </c>
-      <c r="I140" s="40">
+      <c r="I155" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>6</v>
       </c>
-      <c r="J140" s="21" t="str">
+      <c r="J155" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>guayas</v>
       </c>
-      <c r="K140" s="20" t="str">
+      <c r="K155" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>guay</v>
       </c>
-      <c r="L140" s="21" t="str">
+      <c r="L155" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>******</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B141" s="13">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B156" s="13">
         <v>63</v>
       </c>
-      <c r="C141" s="13">
+      <c r="C156" s="13">
         <v>48</v>
       </c>
-      <c r="D141" s="13">
+      <c r="D156" s="13">
         <v>36</v>
       </c>
-      <c r="F141" s="39" t="s">
+      <c r="F156" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G141" s="37" t="str">
+      <c r="G156" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>PASTAZA</v>
       </c>
-      <c r="H141" s="37" t="str">
+      <c r="H156" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>pastaza</v>
       </c>
-      <c r="I141" s="40">
+      <c r="I156" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>7</v>
       </c>
-      <c r="J141" s="21" t="str">
+      <c r="J156" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>pastaza</v>
       </c>
-      <c r="K141" s="20" t="str">
+      <c r="K156" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>past</v>
       </c>
-      <c r="L141" s="21" t="str">
+      <c r="L156" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>*******</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B142" s="13">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B157" s="13">
         <v>35</v>
       </c>
-      <c r="C142" s="13">
+      <c r="C157" s="13">
         <v>28</v>
       </c>
-      <c r="D142" s="13">
+      <c r="D157" s="13">
         <v>25</v>
       </c>
-      <c r="F142" s="39" t="s">
+      <c r="F157" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="G142" s="37" t="str">
+      <c r="G157" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>ESMERALDAS</v>
       </c>
-      <c r="H142" s="37" t="str">
+      <c r="H157" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>esmeraldas</v>
       </c>
-      <c r="I142" s="40">
+      <c r="I157" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>10</v>
       </c>
-      <c r="J142" s="21" t="str">
+      <c r="J157" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>esmeraldas</v>
       </c>
-      <c r="K142" s="20" t="str">
+      <c r="K157" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>esme</v>
       </c>
-      <c r="L142" s="21" t="str">
+      <c r="L157" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>**********</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B143" s="13">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B158" s="13">
         <v>25</v>
       </c>
-      <c r="C143" s="13">
+      <c r="C158" s="13">
         <v>95</v>
       </c>
-      <c r="D143" s="13">
+      <c r="D158" s="13">
         <v>42</v>
       </c>
-      <c r="F143" s="39" t="s">
+      <c r="F158" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="G143" s="37" t="str">
+      <c r="G158" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>LOS RIOS</v>
       </c>
-      <c r="H143" s="37" t="str">
+      <c r="H158" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>los rios</v>
       </c>
-      <c r="I143" s="40">
+      <c r="I158" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>8</v>
       </c>
-      <c r="J143" s="21" t="str">
+      <c r="J158" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>los rios</v>
       </c>
-      <c r="K143" s="20" t="str">
+      <c r="K158" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v xml:space="preserve">los </v>
       </c>
-      <c r="L143" s="21" t="str">
+      <c r="L158" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>********</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A144" s="38" t="s">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A159" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="B144" s="22">
-        <f>MAX(B134:B143)</f>
+      <c r="B159" s="22">
+        <f>MAX(B149:B158)</f>
         <v>84</v>
       </c>
-      <c r="C144" s="22">
-        <f>MAX(C134:C143)</f>
+      <c r="C159" s="22">
+        <f>MAX(C149:C158)</f>
         <v>96</v>
       </c>
-      <c r="D144" s="22">
-        <f>MAX(D134:D143)</f>
+      <c r="D159" s="22">
+        <f>MAX(D149:D158)</f>
         <v>95</v>
       </c>
-      <c r="F144" s="39" t="s">
+      <c r="F159" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="G144" s="37" t="str">
+      <c r="G159" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>MANABI</v>
       </c>
-      <c r="H144" s="37" t="str">
+      <c r="H159" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>manabi</v>
       </c>
-      <c r="I144" s="40">
+      <c r="I159" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>6</v>
       </c>
-      <c r="J144" s="21" t="str">
+      <c r="J159" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>manabi</v>
       </c>
-      <c r="K144" s="20" t="str">
+      <c r="K159" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>mana</v>
       </c>
-      <c r="L144" s="21" t="str">
+      <c r="L159" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>******</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A145" s="38" t="s">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A160" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="B145" s="22">
-        <f>MIN(B134:B143)</f>
+      <c r="B160" s="22">
+        <f>MIN(B149:B158)</f>
         <v>25</v>
       </c>
-      <c r="C145" s="22">
-        <f>MIN(C134:C143)</f>
+      <c r="C160" s="22">
+        <f>MIN(C149:C158)</f>
         <v>28</v>
       </c>
-      <c r="D145" s="22">
-        <f>MIN(D134:D143)</f>
+      <c r="D160" s="22">
+        <f>MIN(D149:D158)</f>
         <v>16</v>
       </c>
-      <c r="F145" s="39" t="s">
+      <c r="F160" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="G145" s="37" t="str">
+      <c r="G160" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>LOJA</v>
       </c>
-      <c r="H145" s="37" t="str">
+      <c r="H160" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>loja</v>
       </c>
-      <c r="I145" s="40">
+      <c r="I160" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>4</v>
       </c>
-      <c r="J145" s="21" t="str">
+      <c r="J160" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>loja</v>
       </c>
-      <c r="K145" s="20" t="str">
+      <c r="K160" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>loja</v>
       </c>
-      <c r="L145" s="21" t="str">
+      <c r="L160" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>****</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F146" s="39" t="s">
+    <row r="161" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F161" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="G146" s="37" t="str">
+      <c r="G161" s="37" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>GALAPAGOS</v>
       </c>
-      <c r="H146" s="37" t="str">
+      <c r="H161" s="37" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>galapagos</v>
       </c>
-      <c r="I146" s="40">
+      <c r="I161" s="40">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>9</v>
       </c>
-      <c r="J146" s="21" t="str">
+      <c r="J161" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>galapagos</v>
       </c>
-      <c r="K146" s="20" t="str">
+      <c r="K161" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>gala</v>
       </c>
-      <c r="L146" s="21" t="str">
+      <c r="L161" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>*********</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B147" s="48" t="s">
+    <row r="162" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B162" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="C147" s="48"/>
-      <c r="F147" s="44" t="s">
+      <c r="C162" s="48"/>
+      <c r="F162" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="G147" s="45" t="str">
+      <c r="G162" s="45" t="str">
         <f>UPPER(Tabla11[[#This Row],[provincias]])</f>
         <v>SANTA ELENA</v>
       </c>
-      <c r="H147" s="45" t="str">
+      <c r="H162" s="45" t="str">
         <f>LOWER(Tabla11[[#This Row],[mayuscula]])</f>
         <v>santa elena</v>
       </c>
-      <c r="I147" s="46">
+      <c r="I162" s="46">
         <f>LEN(Tabla11[[#This Row],[provincias]])</f>
         <v>11</v>
       </c>
-      <c r="J147" s="21" t="str">
+      <c r="J162" s="21" t="str">
         <f>TRIM(Tabla11[[#This Row],[provincias]])</f>
         <v>santa elena</v>
       </c>
-      <c r="K147" s="20" t="str">
+      <c r="K162" s="20" t="str">
         <f>MID(Tabla11[[#This Row],[provincias]],1,4)</f>
         <v>sant</v>
       </c>
-      <c r="L147" s="21" t="str">
+      <c r="L162" s="21" t="str">
         <f>+REPT("*",Tabla11[[#This Row],[num caracteres]])</f>
         <v>***********</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B148" t="s">
+    <row r="163" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B149" t="s">
+    <row r="164" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
         <v>126</v>
       </c>
-      <c r="F149" s="48" t="s">
+      <c r="F164" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="G149" s="48"/>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F150" t="s">
+      <c r="G164" s="48"/>
+    </row>
+    <row r="165" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F165" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F151" t="s">
+    <row r="166" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F166" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F152" t="s">
+    <row r="167" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F167" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F153" s="19" t="s">
+    <row r="168" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F168" s="19" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F154" t="s">
+    <row r="169" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F169" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F155" t="s">
+    <row r="170" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F170" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B162" s="35" t="s">
+    <row r="177" spans="2:12" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B177" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C162" s="35" t="s">
+      <c r="C177" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D162" s="35" t="s">
+      <c r="D177" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E162" s="35" t="s">
+      <c r="E177" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B163" s="35" t="s">
+      <c r="H177" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="I177" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J177" s="53" t="s">
+        <v>216</v>
+      </c>
+      <c r="K177" s="53" t="s">
+        <v>217</v>
+      </c>
+      <c r="L177" s="53" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="178" spans="2:12" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B178" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C163" s="35" t="s">
+      <c r="C178" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D163" s="35" t="s">
+      <c r="D178" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E163" s="35" t="s">
+      <c r="E178" s="4" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B164" s="35" t="s">
+      <c r="H178" s="4">
+        <v>1</v>
+      </c>
+      <c r="I178" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="J178" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K178" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="L178" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="179" spans="2:12" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B179" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C164" s="35" t="s">
+      <c r="C179" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D164" s="35" t="s">
+      <c r="D179" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E164" s="35" t="s">
+      <c r="E179" s="4" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B165" s="35" t="s">
+      <c r="H179" s="4">
+        <v>2</v>
+      </c>
+      <c r="I179" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="J179" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="K179" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="L179" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="180" spans="2:12" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B180" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C165" s="35" t="s">
+      <c r="C180" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D165" s="35" t="s">
+      <c r="D180" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E165" s="35" t="s">
+      <c r="E180" s="4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B166" s="35" t="s">
+      <c r="H180" s="4">
+        <v>3</v>
+      </c>
+      <c r="I180" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="J180" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="K180" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="L180" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="181" spans="2:12" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B181" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C166" s="35" t="s">
+      <c r="C181" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D166" s="35" t="s">
+      <c r="D181" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="E166" s="35" t="s">
+      <c r="E181" s="4" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B167" s="35" t="s">
+      <c r="H181" s="4">
+        <v>4</v>
+      </c>
+      <c r="I181" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="J181" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K181" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="L181" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="182" spans="2:12" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B182" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C167" s="35" t="s">
+      <c r="C182" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="D167" s="35" t="s">
+      <c r="D182" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E167" s="35" t="s">
+      <c r="E182" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B168" s="35" t="s">
+      <c r="H182" s="4">
+        <v>5</v>
+      </c>
+      <c r="I182" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="J182" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="K182" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="L182" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="183" spans="2:12" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B183" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C168" s="35" t="s">
+      <c r="C183" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D168" s="35" t="s">
+      <c r="D183" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="E168" s="35" t="s">
+      <c r="E183" s="4" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B169" s="35" t="s">
+      <c r="H183" s="4">
+        <v>6</v>
+      </c>
+      <c r="I183" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="J183" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="K183" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="L183" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="184" spans="2:12" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B184" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C169" s="35" t="s">
+      <c r="C184" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D169" s="35" t="s">
+      <c r="D184" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E169" s="35" t="s">
+      <c r="E184" s="4" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B170" s="35" t="s">
+      <c r="H184" s="4">
+        <v>7</v>
+      </c>
+      <c r="I184" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="J184" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="K184" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L184" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="185" spans="2:12" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B185" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C170" s="35" t="s">
+      <c r="C185" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D170" s="35" t="s">
+      <c r="D185" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="E170" s="35" t="s">
+      <c r="E185" s="4" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B171" s="35" t="s">
+      <c r="H185" s="4">
+        <v>8</v>
+      </c>
+      <c r="I185" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="J185" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="K185" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="L185" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="186" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B186" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="C171" s="35" t="s">
+      <c r="C186" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="D171" s="35" t="s">
+      <c r="D186" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="E171" s="35" t="s">
+      <c r="E186" s="35" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B173" s="47" t="s">
+    <row r="187" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H187" s="54"/>
+      <c r="I187" s="55" t="s">
+        <v>219</v>
+      </c>
+      <c r="J187" s="56" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="188" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B188" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="C173" s="47"/>
-      <c r="D173" s="47"/>
-      <c r="E173" s="47"/>
-      <c r="F173" s="47"/>
-    </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B174" t="s">
+      <c r="C188" s="47"/>
+      <c r="D188" s="47"/>
+      <c r="E188" s="47"/>
+      <c r="F188" s="47"/>
+      <c r="H188" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="I188" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="J188" s="57">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="189" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
         <v>189</v>
+      </c>
+      <c r="H189" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="I189" s="58">
+        <f>MATCH(I188,Tabla13[Nombre vendedor],)</f>
+        <v>6</v>
+      </c>
+      <c r="J189" t="e">
+        <f>MATCH(J188,Tabla13[[#Headers],[2020]:[2022]],)</f>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B173:F173"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="E126:F126"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="H130:I130"/>
-    <mergeCell ref="K130:L130"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="F149:G149"/>
-    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B17:L17"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B188:F188"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B141:C141"/>
+    <mergeCell ref="E141:F141"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="H145:I145"/>
+    <mergeCell ref="K145:L145"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="F164:G164"/>
+    <mergeCell ref="F98:H98"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="G4:J5">
-    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="hubo perdidas">
-      <formula>NOT(ISERROR(SEARCH("hubo perdidas",G4)))</formula>
+  <conditionalFormatting sqref="G19:J20">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="hubo perdidas">
+      <formula>NOT(ISERROR(SEARCH("hubo perdidas",G19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="hubo perdidas">
-      <formula>NOT(ISERROR(SEARCH("hubo perdidas",G4)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="hubo perdidas">
+      <formula>NOT(ISERROR(SEARCH("hubo perdidas",G19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:J9">
-    <cfRule type="containsText" dxfId="77" priority="3" operator="containsText" text="hubo beneficios">
-      <formula>NOT(ISERROR(SEARCH("hubo beneficios",G4)))</formula>
+  <conditionalFormatting sqref="G19:J24">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="hubo beneficios">
+      <formula>NOT(ISERROR(SEARCH("hubo beneficios",G19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="4" operator="containsText" text="hubo perdidas">
-      <formula>NOT(ISERROR(SEARCH("hubo perdidas",G4)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="hubo perdidas">
+      <formula>NOT(ISERROR(SEARCH("hubo perdidas",G19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L4:L9">
-    <cfRule type="containsText" dxfId="75" priority="1" operator="containsText" text="no hubo beneficios en todos los trimestres">
-      <formula>NOT(ISERROR(SEARCH("no hubo beneficios en todos los trimestres",L4)))</formula>
+  <conditionalFormatting sqref="L19:L24">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no hubo beneficios en todos los trimestres">
+      <formula>NOT(ISERROR(SEARCH("no hubo beneficios en todos los trimestres",L19)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"beneficios en los tres trimestres"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1" xr:uid="{60CE2398-C382-4788-931D-C6DBA2483FDB}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{4AA26A06-29B4-43DB-B556-B711F3AE47C4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="12">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <tableParts count="13">
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
@@ -4828,6 +5194,9 @@
     <tablePart r:id="rId11"/>
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>